<commit_message>
Lab 02: Added prezenta laborator. Added solution to database problem.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="87">
   <si>
     <t>Nr.</t>
   </si>
@@ -197,6 +197,90 @@
   </si>
   <si>
     <t>Dulau I. Marius Cristian (mutat gr 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeic E. Naomi Ioana </t>
+  </si>
+  <si>
+    <t>Tema 1</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Chatroom</t>
+  </si>
+  <si>
+    <t>Inchiriere masini Android</t>
+  </si>
+  <si>
+    <t>Magazin e commerce</t>
+  </si>
+  <si>
+    <t>Nutritie</t>
+  </si>
+  <si>
+    <t>Librarie online</t>
+  </si>
+  <si>
+    <t>Aplicatie pontaj</t>
+  </si>
+  <si>
+    <t>Tema proiect final</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>P  *</t>
+  </si>
+  <si>
+    <t>P *</t>
+  </si>
+  <si>
+    <t>* activitate la laborator</t>
+  </si>
+  <si>
+    <t>Hotel management</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>Inchiriere de masini</t>
+  </si>
+  <si>
+    <t>Comenzi restaurant</t>
+  </si>
+  <si>
+    <t>Liga fotbal</t>
+  </si>
+  <si>
+    <t>Agentie turism</t>
+  </si>
+  <si>
+    <t>Restaurant tips application</t>
+  </si>
+  <si>
+    <t>Employee resource management</t>
+  </si>
+  <si>
+    <t>Saloon reservation management</t>
+  </si>
+  <si>
+    <t>Online job manager</t>
+  </si>
+  <si>
+    <t>Gestionare/plata amenzi</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>Ticketing application</t>
   </si>
 </sst>
 </file>
@@ -396,7 +480,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -415,6 +517,42 @@
           <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -467,14 +605,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="firstRowStripe" dxfId="9"/>
+      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+    </tableStyle>
+    <tableStyle name="attendance-style" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
       <tableStyleElement type="secondRowStripe" dxfId="5"/>
-    </tableStyle>
-    <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -489,8 +627,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:R39">
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:U39">
+  <tableColumns count="21">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
     <tableColumn id="3" name="L01"/>
@@ -509,6 +647,9 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="4"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="0"/>
+    <tableColumn id="21" name="Column1" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -802,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -813,7 +954,10 @@
     <col min="3" max="16" width="7.140625" customWidth="1"/>
     <col min="17" max="17" width="19.140625" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" customWidth="1"/>
-    <col min="19" max="27" width="7.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" customWidth="1"/>
+    <col min="21" max="21" width="24" customWidth="1"/>
+    <col min="22" max="27" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
@@ -871,9 +1015,15 @@
       <c r="R1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="S1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
@@ -892,7 +1042,9 @@
       <c r="C2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E2" s="17"/>
       <c r="F2" s="14"/>
       <c r="G2" s="17"/>
@@ -907,11 +1059,15 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2" s="17"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
+      <c r="S2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
@@ -931,7 +1087,9 @@
       <c r="C3" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="21"/>
+      <c r="D3" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -946,11 +1104,15 @@
       <c r="P3" s="21"/>
       <c r="Q3" s="17">
         <f t="shared" ref="Q3:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3" s="21"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
+      <c r="S3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
@@ -959,7 +1121,7 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+    <row r="4" spans="1:27" ht="15.75" hidden="1" customHeight="1">
       <c r="A4" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -985,8 +1147,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R4" s="17"/>
-      <c r="S4" s="10"/>
+      <c r="R4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
@@ -996,7 +1162,7 @@
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1">
+    <row r="5" spans="1:27">
       <c r="A5" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1007,7 +1173,9 @@
       <c r="C5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -1022,11 +1190,15 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R5" s="21"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
+      <c r="S5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>80</v>
+      </c>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -1035,7 +1207,7 @@
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1">
+    <row r="6" spans="1:27" hidden="1">
       <c r="A6" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1063,8 +1235,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R6" s="17"/>
-      <c r="S6" s="10"/>
+      <c r="R6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
@@ -1085,7 +1261,9 @@
       <c r="C7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -1100,11 +1278,15 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="21"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
+      <c r="S7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -1124,7 +1306,9 @@
       <c r="C8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -1139,11 +1323,15 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="17"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
+      <c r="S8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -1163,7 +1351,9 @@
       <c r="C9" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -1178,11 +1368,15 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="21"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
+      <c r="S9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -1202,7 +1396,9 @@
       <c r="C10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -1217,11 +1413,15 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="17"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
+      <c r="S10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
@@ -1241,7 +1441,9 @@
       <c r="C11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -1256,11 +1458,15 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" s="21"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
+      <c r="S11" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T11" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -1280,7 +1486,9 @@
       <c r="C12" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="27"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -1295,11 +1503,15 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" s="17"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
+      <c r="S12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T12" s="10" t="s">
+        <v>76</v>
+      </c>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
@@ -1319,7 +1531,9 @@
       <c r="C13" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
@@ -1334,11 +1548,15 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" s="21"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
+      <c r="S13" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -1358,7 +1576,9 @@
       <c r="C14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
@@ -1373,11 +1593,15 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" s="17"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
+      <c r="S14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -1397,7 +1621,9 @@
       <c r="C15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
@@ -1412,11 +1638,15 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="21"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
+      <c r="S15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
@@ -1436,7 +1666,9 @@
       <c r="C16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="17"/>
+      <c r="D16" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -1451,11 +1683,15 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" s="17"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
+      <c r="S16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -1475,7 +1711,9 @@
       <c r="C17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E17" s="21"/>
       <c r="F17" s="26"/>
       <c r="G17" s="21"/>
@@ -1490,11 +1728,15 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R17" s="21"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
+      <c r="S17" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>67</v>
+      </c>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
@@ -1503,7 +1745,7 @@
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
     </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1">
+    <row r="18" spans="1:27" ht="15.75" hidden="1" customHeight="1">
       <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1531,7 +1773,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R18" s="17"/>
+      <c r="R18" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
@@ -1553,7 +1797,9 @@
       <c r="C19" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -1568,11 +1814,15 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="21"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
+      <c r="S19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
@@ -1592,7 +1842,9 @@
       <c r="C20" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -1607,11 +1859,15 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R20" s="17"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
+      <c r="S20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
@@ -1620,7 +1876,7 @@
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1">
+    <row r="21" spans="1:27" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1646,7 +1902,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R21" s="21"/>
+      <c r="R21" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
@@ -1668,7 +1926,9 @@
       <c r="C22" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -1683,11 +1943,15 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R22" s="17"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
+      <c r="S22" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T22" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
@@ -1696,7 +1960,7 @@
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
     </row>
-    <row r="23" spans="1:27" ht="15.75" customHeight="1">
+    <row r="23" spans="1:27">
       <c r="A23" s="19">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1707,7 +1971,9 @@
       <c r="C23" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="21"/>
+      <c r="D23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
@@ -1722,11 +1988,15 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R23" s="21"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
+      <c r="S23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -1735,7 +2005,7 @@
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
     </row>
-    <row r="24" spans="1:27" ht="15.75" customHeight="1">
+    <row r="24" spans="1:27" ht="15.75" hidden="1" customHeight="1">
       <c r="A24" s="11">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1763,7 +2033,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R24" s="17"/>
+      <c r="R24" s="17" t="s">
+        <v>62</v>
+      </c>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
@@ -1774,13 +2046,13 @@
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
     </row>
-    <row r="25" spans="1:27" ht="15.75" customHeight="1">
+    <row r="25" spans="1:27" hidden="1">
       <c r="A25" s="19">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="21"/>
@@ -1800,7 +2072,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R25" s="21"/>
+      <c r="R25" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
       <c r="U25" s="10"/>
@@ -1821,7 +2095,9 @@
       <c r="C26" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -1837,7 +2113,9 @@
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
       <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
+      <c r="T26" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
@@ -1964,7 +2242,9 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="19"/>
-      <c r="B31" s="30"/>
+      <c r="B31" s="30" t="s">
+        <v>73</v>
+      </c>
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
@@ -2225,13 +2505,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:P39">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2240,7 +2521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3531,7 +3814,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L39 M2:M39">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 03: Added prezenta.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
   <si>
     <t>Nr.</t>
   </si>
@@ -281,13 +281,19 @@
   </si>
   <si>
     <t>Ticketing application</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>P*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -317,8 +323,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +347,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFD7D7D7"/>
       </patternFill>
     </fill>
   </fills>
@@ -365,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -476,45 +500,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -553,6 +560,35 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -647,9 +683,9 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="4"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="0"/>
-    <tableColumn id="21" name="Column1" dataDxfId="3"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="3"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="2"/>
+    <tableColumn id="21" name="Column1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -943,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1045,7 +1081,9 @@
       <c r="D2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F2" s="14"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
@@ -1059,7 +1097,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1090,7 +1128,9 @@
       <c r="D3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -1104,7 +1144,7 @@
       <c r="P3" s="21"/>
       <c r="Q3" s="17">
         <f t="shared" ref="Q3:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="10" t="s">
@@ -1176,7 +1216,9 @@
       <c r="D5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
@@ -1190,7 +1232,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1264,7 +1306,9 @@
       <c r="D7" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
@@ -1278,7 +1322,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1309,7 +1353,9 @@
       <c r="D8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -1323,7 +1369,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1354,7 +1400,9 @@
       <c r="D9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -1368,7 +1416,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1399,7 +1447,9 @@
       <c r="D10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="42" t="s">
+        <v>87</v>
+      </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -1413,7 +1463,7 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="10" t="s">
@@ -1444,7 +1494,9 @@
       <c r="D11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
@@ -1458,7 +1510,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1489,7 +1541,9 @@
       <c r="D12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -1503,7 +1557,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
@@ -1534,7 +1588,9 @@
       <c r="D13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
@@ -1548,7 +1604,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1579,7 +1635,9 @@
       <c r="D14" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1593,7 +1651,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1624,7 +1682,9 @@
       <c r="D15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
@@ -1638,7 +1698,7 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="10" t="s">
@@ -1669,7 +1729,9 @@
       <c r="D16" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
@@ -1683,7 +1745,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1714,7 +1776,9 @@
       <c r="D17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="F17" s="26"/>
       <c r="G17" s="21"/>
       <c r="H17" s="26"/>
@@ -1728,7 +1792,7 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -1800,7 +1864,9 @@
       <c r="D19" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="21"/>
+      <c r="E19" s="44" t="s">
+        <v>88</v>
+      </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
@@ -1814,7 +1880,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -1845,7 +1911,9 @@
       <c r="D20" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="45" t="s">
+        <v>88</v>
+      </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -1859,7 +1927,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -1929,7 +1997,9 @@
       <c r="D22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -1943,7 +2013,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -1974,7 +2044,9 @@
       <c r="D23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
@@ -1988,7 +2060,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2098,7 +2170,9 @@
       <c r="D26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="17"/>
@@ -2112,7 +2186,9 @@
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
-      <c r="S26" s="10"/>
+      <c r="S26" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="T26" s="10" t="s">
         <v>79</v>
       </c>
@@ -2505,7 +2581,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:P39">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2521,7 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -3814,7 +3890,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L39 M2:M39">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 04: Added note documentatie.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="90">
   <si>
     <t>Nr.</t>
   </si>
@@ -283,10 +283,13 @@
     <t>Ticketing application</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>P*</t>
+  </si>
+  <si>
+    <t>Bompa Flaviu</t>
+  </si>
+  <si>
+    <t>Microservicii vs SOA</t>
   </si>
 </sst>
 </file>
@@ -516,12 +519,34 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -581,14 +606,21 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -641,14 +673,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -683,17 +715,17 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="3"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="2"/>
-    <tableColumn id="21" name="Column1" dataDxfId="1"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="6"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="5"/>
+    <tableColumn id="21" name="Column1" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:O39">
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:P39">
+  <tableColumns count="16">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
     <tableColumn id="3" name="H1"/>
@@ -709,6 +741,7 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1084,8 +1117,10 @@
       <c r="E2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="35"/>
       <c r="H2" s="17"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17"/>
@@ -1097,7 +1132,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1129,10 +1164,10 @@
         <v>72</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+        <v>87</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
@@ -1173,7 +1208,7 @@
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -1219,8 +1254,10 @@
       <c r="E5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="26"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
@@ -1232,7 +1269,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1263,7 +1300,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -1307,10 +1344,12 @@
         <v>72</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+        <v>87</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="26"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
@@ -1322,7 +1361,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1356,8 +1395,10 @@
       <c r="E8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="F8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="35"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -1369,7 +1410,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1401,10 +1442,10 @@
         <v>54</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+        <v>87</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -1447,11 +1488,9 @@
       <c r="D10" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -1463,7 +1502,7 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="10" t="s">
@@ -1497,8 +1536,10 @@
       <c r="E11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="26"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
@@ -1510,7 +1551,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1544,8 +1585,8 @@
       <c r="E12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -1591,8 +1632,10 @@
       <c r="E13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="26"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
@@ -1604,7 +1647,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1638,8 +1681,10 @@
       <c r="E14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="F14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="35"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -1651,7 +1696,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1682,11 +1727,9 @@
       <c r="D15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="26"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
@@ -1698,7 +1741,7 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="10" t="s">
@@ -1732,8 +1775,10 @@
       <c r="E16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="F16" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="35"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -1745,7 +1790,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1779,8 +1824,10 @@
       <c r="E17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="26"/>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
       <c r="J17" s="26"/>
@@ -1792,7 +1839,7 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -1823,7 +1870,7 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -1865,10 +1912,12 @@
         <v>71</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
+        <v>87</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="26"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
@@ -1880,7 +1929,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -1912,10 +1961,12 @@
         <v>71</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+        <v>87</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="35"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -1927,7 +1978,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -1956,7 +2007,7 @@
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
@@ -2000,8 +2051,10 @@
       <c r="E22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="35"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -2013,7 +2066,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2047,8 +2100,10 @@
       <c r="E23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
+      <c r="F23" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="26"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
@@ -2060,7 +2115,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2091,7 +2146,7 @@
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
@@ -2130,7 +2185,7 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
@@ -2173,8 +2228,10 @@
       <c r="E26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="35"/>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
@@ -2580,9 +2637,14 @@
       <c r="AA39" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:P39">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+  <conditionalFormatting sqref="C27:P39 H2:P26 C2:F26">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(C2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G26">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2597,8 +2659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2608,14 +2670,15 @@
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="7" width="6.85546875" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="6.140625" customWidth="1"/>
     <col min="10" max="10" width="5.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="14" width="18.7109375" customWidth="1"/>
     <col min="15" max="15" width="73.140625" customWidth="1"/>
-    <col min="16" max="21" width="7.5703125" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="21" width="7.5703125" customWidth="1"/>
     <col min="22" max="23" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2665,7 +2728,9 @@
       <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="9"/>
+      <c r="P1" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
@@ -2687,17 +2752,19 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
-      <c r="H2" s="15"/>
+      <c r="H2" s="15">
+        <v>9</v>
+      </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16">
-        <f t="shared" ref="L2:L25" si="1">(E2 + F2 + G2)/3</f>
+        <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
         <v>0</v>
       </c>
       <c r="M2" s="15">
-        <f t="shared" ref="M2:M25" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
-        <v>0</v>
+        <f>(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
+        <v>0.9</v>
       </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
@@ -2732,7 +2799,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="15">
-        <f t="shared" si="2"/>
+        <f>(H3/10 +I3/10 + J3/10 + K3*7/10)</f>
         <v>0</v>
       </c>
       <c r="N3" s="18"/>
@@ -2746,7 +2813,7 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1">
+    <row r="4" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A4" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2768,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="15">
-        <f t="shared" si="2"/>
+        <f>(H4/10 +I4/10 + J4/10 + K4*7/10)</f>
         <v>0</v>
       </c>
       <c r="N4" s="18"/>
@@ -2795,7 +2862,9 @@
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="23">
+        <v>10</v>
+      </c>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
       <c r="K5" s="16"/>
@@ -2804,12 +2873,14 @@
         <v>0</v>
       </c>
       <c r="M5" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H5/10 +I5/10 + J5/10 + K5*7/10)</f>
+        <v>1</v>
       </c>
       <c r="N5" s="24"/>
       <c r="O5" s="25"/>
-      <c r="P5" s="10"/>
+      <c r="P5" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
@@ -2818,7 +2889,7 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1">
+    <row r="6" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A6" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2840,7 +2911,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="15">
-        <f t="shared" si="2"/>
+        <f>(H6/10 +I6/10 + J6/10 + K6*7/10)</f>
         <v>0</v>
       </c>
       <c r="N6" s="25"/>
@@ -2867,7 +2938,9 @@
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
+      <c r="H7" s="23">
+        <v>10</v>
+      </c>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
       <c r="K7" s="16"/>
@@ -2876,12 +2949,14 @@
         <v>0</v>
       </c>
       <c r="M7" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H7/10 +I7/10 + J7/10 + K7*7/10)</f>
+        <v>1</v>
       </c>
       <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
@@ -2903,7 +2978,9 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
+      <c r="H8" s="23">
+        <v>10</v>
+      </c>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
       <c r="K8" s="16"/>
@@ -2912,12 +2989,14 @@
         <v>0</v>
       </c>
       <c r="M8" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H8/10 +I8/10 + J8/10 + K8*7/10)</f>
+        <v>1</v>
       </c>
       <c r="N8" s="24"/>
       <c r="O8" s="25"/>
-      <c r="P8" s="10"/>
+      <c r="P8" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
@@ -2948,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="15">
-        <f t="shared" si="2"/>
+        <f>(H9/10 +I9/10 + J9/10 + K9*7/10)</f>
         <v>0</v>
       </c>
       <c r="N9" s="18"/>
@@ -2984,7 +3063,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="15">
-        <f t="shared" si="2"/>
+        <f>(H10/10 +I10/10 + J10/10 + K10*7/10)</f>
         <v>0</v>
       </c>
       <c r="N10" s="18"/>
@@ -3011,7 +3090,9 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="15"/>
+      <c r="H11" s="15">
+        <v>10</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="16"/>
@@ -3020,12 +3101,14 @@
         <v>0</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H11/10 +I11/10 + J11/10 + K11*7/10)</f>
+        <v>1</v>
       </c>
       <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="10"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
@@ -3056,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="15">
-        <f t="shared" si="2"/>
+        <f>(H12/10 +I12/10 + J12/10 + K12*7/10)</f>
         <v>0</v>
       </c>
       <c r="N12" s="18"/>
@@ -3083,7 +3166,9 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+      <c r="H13" s="23">
+        <v>9.5</v>
+      </c>
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
       <c r="K13" s="16"/>
@@ -3092,8 +3177,8 @@
         <v>0</v>
       </c>
       <c r="M13" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H13/10 +I13/10 + J13/10 + K13*7/10)</f>
+        <v>0.95</v>
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -3119,7 +3204,9 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="15">
+        <v>8</v>
+      </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
       <c r="K14" s="16"/>
@@ -3128,12 +3215,14 @@
         <v>0</v>
       </c>
       <c r="M14" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H14/10 +I14/10 + J14/10 + K14*7/10)</f>
+        <v>0.8</v>
       </c>
       <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="10"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
@@ -3164,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="15">
-        <f t="shared" si="2"/>
+        <f>(H15/10 +I15/10 + J15/10 + K15*7/10)</f>
         <v>0</v>
       </c>
       <c r="N15" s="25"/>
@@ -3191,7 +3280,9 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="15">
+        <v>6</v>
+      </c>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
       <c r="K16" s="16"/>
@@ -3200,12 +3291,14 @@
         <v>0</v>
       </c>
       <c r="M16" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H16/10 +I16/10 + J16/10 + K16*7/10)</f>
+        <v>0.6</v>
       </c>
       <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="10"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -3227,7 +3320,9 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
+      <c r="H17" s="23">
+        <v>9</v>
+      </c>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
       <c r="K17" s="16"/>
@@ -3236,12 +3331,14 @@
         <v>0</v>
       </c>
       <c r="M17" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H17/10 +I17/10 + J17/10 + K17*7/10)</f>
+        <v>0.9</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
-      <c r="P17" s="10"/>
+      <c r="P17" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
@@ -3250,7 +3347,7 @@
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1">
+    <row r="18" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A18" s="11">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3272,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="15">
-        <f t="shared" si="2"/>
+        <f>(H18/10 +I18/10 + J18/10 + K18*7/10)</f>
         <v>0</v>
       </c>
       <c r="N18" s="18"/>
@@ -3299,7 +3396,9 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="15">
+        <v>10</v>
+      </c>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
       <c r="K19" s="16"/>
@@ -3308,12 +3407,14 @@
         <v>0</v>
       </c>
       <c r="M19" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H19/10 +I19/10 + J19/10 + K19*7/10)</f>
+        <v>1</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
-      <c r="P19" s="10"/>
+      <c r="P19" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
@@ -3335,7 +3436,9 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="15"/>
+      <c r="H20" s="15">
+        <v>9</v>
+      </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
       <c r="K20" s="16"/>
@@ -3344,12 +3447,14 @@
         <v>0</v>
       </c>
       <c r="M20" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H20/10 +I20/10 + J20/10 + K20*7/10)</f>
+        <v>0.9</v>
       </c>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
-      <c r="P20" s="10"/>
+      <c r="P20" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
@@ -3358,7 +3463,7 @@
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1">
+    <row r="21" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3380,7 +3485,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="15">
-        <f t="shared" si="2"/>
+        <f>(H21/10 +I21/10 + J21/10 + K21*7/10)</f>
         <v>0</v>
       </c>
       <c r="N21" s="18"/>
@@ -3407,7 +3512,9 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
+      <c r="H22" s="23">
+        <v>9</v>
+      </c>
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
       <c r="K22" s="16"/>
@@ -3416,12 +3523,14 @@
         <v>0</v>
       </c>
       <c r="M22" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H22/10 +I22/10 + J22/10 + K22*7/10)</f>
+        <v>0.9</v>
       </c>
       <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="10"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
@@ -3443,7 +3552,9 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="15"/>
+      <c r="H23" s="15">
+        <v>7</v>
+      </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
@@ -3452,12 +3563,14 @@
         <v>0</v>
       </c>
       <c r="M23" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(H23/10 +I23/10 + J23/10 + K23*7/10)</f>
+        <v>0.7</v>
       </c>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
-      <c r="P23" s="10"/>
+      <c r="P23" s="10">
+        <v>0.2</v>
+      </c>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
@@ -3466,7 +3579,7 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" customHeight="1">
+    <row r="24" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A24" s="11">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3487,8 +3600,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M24" s="15">
-        <f t="shared" si="2"/>
+      <c r="M24" s="23">
+        <f>(H24/10 +I24/10 + J24/10 + K24*7/10)</f>
         <v>0</v>
       </c>
       <c r="N24" s="18"/>
@@ -3502,7 +3615,7 @@
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" spans="1:23" ht="15.75" customHeight="1">
+    <row r="25" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A25" s="19">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3523,8 +3636,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="15">
-        <f t="shared" si="2"/>
+      <c r="M25" s="23">
+        <f>(H25/10 +I25/10 + J25/10 + K25*7/10)</f>
         <v>0</v>
       </c>
       <c r="N25" s="18"/>
@@ -3539,19 +3652,31 @@
       <c r="W25" s="10"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="18">
+        <v>23</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="15"/>
+      <c r="H26" s="15">
+        <v>9</v>
+      </c>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="15"/>
+      <c r="L26" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="23">
+        <f>(H26/10 +I26/10 + J26/10 + K26*7/10)</f>
+        <v>0.9</v>
+      </c>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
       <c r="P26" s="10"/>
@@ -3889,7 +4014,7 @@
       <c r="W39" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L2:L39 M2:M39">
+  <conditionalFormatting sqref="L2:M39">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>

</xml_diff>

<commit_message>
Lab 05: Added grades Assignment1.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="90">
   <si>
     <t>Nr.</t>
   </si>
@@ -521,32 +521,28 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -606,21 +602,25 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -715,9 +715,9 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="6"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="5"/>
-    <tableColumn id="21" name="Column1" dataDxfId="4"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="4"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="3"/>
+    <tableColumn id="21" name="Column1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -741,7 +741,7 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="3"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1120,7 +1120,9 @@
       <c r="F2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="35"/>
+      <c r="G2" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H2" s="17"/>
       <c r="I2" s="14"/>
       <c r="J2" s="17"/>
@@ -1132,7 +1134,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1257,7 +1259,9 @@
       <c r="F5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
@@ -1269,7 +1273,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1349,7 +1353,9 @@
       <c r="F7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
@@ -1361,7 +1367,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1445,7 +1451,9 @@
         <v>87</v>
       </c>
       <c r="F9" s="43"/>
-      <c r="G9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
@@ -1457,7 +1465,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1539,7 +1547,9 @@
       <c r="F11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21"/>
@@ -1551,7 +1561,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1586,7 +1596,9 @@
         <v>54</v>
       </c>
       <c r="F12" s="42"/>
-      <c r="G12" s="35"/>
+      <c r="G12" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -1598,7 +1610,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
@@ -1635,7 +1647,9 @@
       <c r="F13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="26"/>
+      <c r="G13" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="21"/>
@@ -1647,7 +1661,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1684,7 +1698,9 @@
       <c r="F14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="35"/>
+      <c r="G14" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -1696,7 +1712,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1778,7 +1794,9 @@
       <c r="F16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="35"/>
+      <c r="G16" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
@@ -1790,7 +1808,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1917,7 +1935,9 @@
       <c r="F19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="26"/>
+      <c r="G19" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
       <c r="J19" s="21"/>
@@ -1929,7 +1949,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -1966,7 +1986,9 @@
       <c r="F20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="35"/>
+      <c r="G20" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -1978,7 +2000,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2054,7 +2076,9 @@
       <c r="F22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="35"/>
+      <c r="G22" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -2066,7 +2090,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2103,7 +2127,9 @@
       <c r="F23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
@@ -2115,7 +2141,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2231,7 +2257,9 @@
       <c r="F26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="35"/>
+      <c r="G26" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
@@ -2638,12 +2666,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C27:P39 H2:P26 C2:F26">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="6" priority="2">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G26">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2659,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2763,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="15">
-        <f>(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
+        <f t="shared" ref="M2:M26" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
         <v>0.9</v>
       </c>
       <c r="N2" s="18"/>
@@ -2799,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="15">
-        <f>(H3/10 +I3/10 + J3/10 + K3*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N3" s="18"/>
@@ -2835,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="15">
-        <f>(H4/10 +I4/10 + J4/10 + K4*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N4" s="18"/>
@@ -2859,7 +2887,9 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="22"/>
+      <c r="E5" s="22">
+        <v>9.5</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23">
@@ -2870,10 +2900,10 @@
       <c r="K5" s="16"/>
       <c r="L5" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="M5" s="15">
-        <f>(H5/10 +I5/10 + J5/10 + K5*7/10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N5" s="24"/>
@@ -2911,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="15">
-        <f>(H6/10 +I6/10 + J6/10 + K6*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N6" s="25"/>
@@ -2935,7 +2965,9 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="22"/>
+      <c r="E7" s="22">
+        <v>10</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="23">
@@ -2946,10 +2978,10 @@
       <c r="K7" s="16"/>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="M7" s="15">
-        <f>(H7/10 +I7/10 + J7/10 + K7*7/10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N7" s="18"/>
@@ -2989,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="15">
-        <f>(H8/10 +I8/10 + J8/10 + K8*7/10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N8" s="24"/>
@@ -3015,7 +3047,9 @@
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="22">
+        <v>9.5</v>
+      </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="15"/>
@@ -3024,10 +3058,10 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.1666666666666665</v>
       </c>
       <c r="M9" s="15">
-        <f>(H9/10 +I9/10 + J9/10 + K9*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N9" s="18"/>
@@ -3063,7 +3097,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="15">
-        <f>(H10/10 +I10/10 + J10/10 + K10*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N10" s="18"/>
@@ -3087,7 +3121,9 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="22"/>
+      <c r="E11" s="22">
+        <v>10</v>
+      </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="15">
@@ -3098,10 +3134,10 @@
       <c r="K11" s="16"/>
       <c r="L11" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="M11" s="15">
-        <f>(H11/10 +I11/10 + J11/10 + K11*7/10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N11" s="18"/>
@@ -3139,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="15">
-        <f>(H12/10 +I12/10 + J12/10 + K12*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N12" s="18"/>
@@ -3177,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="15">
-        <f>(H13/10 +I13/10 + J13/10 + K13*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.95</v>
       </c>
       <c r="N13" s="18"/>
@@ -3215,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="15">
-        <f>(H14/10 +I14/10 + J14/10 + K14*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="N14" s="18"/>
@@ -3253,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="15">
-        <f>(H15/10 +I15/10 + J15/10 + K15*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N15" s="25"/>
@@ -3277,7 +3313,9 @@
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="22"/>
+      <c r="E16" s="22">
+        <v>8.5</v>
+      </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="15">
@@ -3288,10 +3326,10 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="M16" s="15">
-        <f>(H16/10 +I16/10 + J16/10 + K16*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="N16" s="18"/>
@@ -3331,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="15">
-        <f>(H17/10 +I17/10 + J17/10 + K17*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="N17" s="18"/>
@@ -3369,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="15">
-        <f>(H18/10 +I18/10 + J18/10 + K18*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N18" s="18"/>
@@ -3393,7 +3431,9 @@
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="22"/>
+      <c r="E19" s="22">
+        <v>10</v>
+      </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
       <c r="H19" s="15">
@@ -3404,10 +3444,10 @@
       <c r="K19" s="16"/>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="M19" s="15">
-        <f>(H19/10 +I19/10 + J19/10 + K19*7/10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N19" s="18"/>
@@ -3433,7 +3473,9 @@
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="22"/>
+      <c r="E20" s="22">
+        <v>8.5</v>
+      </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="15">
@@ -3444,10 +3486,10 @@
       <c r="K20" s="16"/>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.8333333333333335</v>
       </c>
       <c r="M20" s="15">
-        <f>(H20/10 +I20/10 + J20/10 + K20*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="N20" s="18"/>
@@ -3485,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="15">
-        <f>(H21/10 +I21/10 + J21/10 + K21*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N21" s="18"/>
@@ -3523,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="15">
-        <f>(H22/10 +I22/10 + J22/10 + K22*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="N22" s="18"/>
@@ -3563,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="15">
-        <f>(H23/10 +I23/10 + J23/10 + K23*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
       <c r="N23" s="18"/>
@@ -3601,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="23">
-        <f>(H24/10 +I24/10 + J24/10 + K24*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N24" s="18"/>
@@ -3637,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="23">
-        <f>(H25/10 +I25/10 + J25/10 + K25*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N25" s="18"/>
@@ -3674,7 +3716,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="23">
-        <f>(H26/10 +I26/10 + J26/10 + K26*7/10)</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="N26" s="18"/>
@@ -4015,7 +4057,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M39">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 07: Added grades Assignment1 and PD2
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="91">
   <si>
     <t>Nr.</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Microservicii vs SOA</t>
+  </si>
+  <si>
+    <t>Builder Pattern</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -673,14 +712,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="secondRowStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -715,17 +754,17 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="4"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="3"/>
-    <tableColumn id="21" name="Column1" dataDxfId="2"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="6"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="5"/>
+    <tableColumn id="21" name="Column1" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:P39">
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:R39">
+  <tableColumns count="18">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
     <tableColumn id="3" name="H1"/>
@@ -741,7 +780,9 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="0"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="2"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="1"/>
+    <tableColumn id="18" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1012,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1123,8 +1164,9 @@
       <c r="G2" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="14"/>
+      <c r="I2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="14"/>
@@ -1134,7 +1176,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1170,8 +1212,9 @@
       </c>
       <c r="F3" s="43"/>
       <c r="G3" s="26"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="I3" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
@@ -1181,7 +1224,7 @@
       <c r="P3" s="21"/>
       <c r="Q3" s="17">
         <f t="shared" ref="Q3:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="10" t="s">
@@ -1211,7 +1254,6 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="35"/>
-      <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
@@ -1262,8 +1304,9 @@
       <c r="G5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="I5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
@@ -1273,7 +1316,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1305,7 +1348,6 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="35"/>
-      <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
@@ -1356,8 +1398,9 @@
       <c r="G7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="I7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
@@ -1367,7 +1410,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1405,8 +1448,9 @@
         <v>54</v>
       </c>
       <c r="G8" s="35"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="I8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
@@ -1416,7 +1460,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1454,8 +1498,9 @@
       <c r="G9" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -1465,7 +1510,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1499,7 +1544,6 @@
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1550,8 +1594,9 @@
       <c r="G11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="I11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
@@ -1561,7 +1606,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1599,8 +1644,9 @@
       <c r="G12" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="I12" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
@@ -1610,7 +1656,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
@@ -1650,8 +1696,9 @@
       <c r="G13" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="I13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
@@ -1661,7 +1708,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1701,8 +1748,9 @@
       <c r="G14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="I14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
@@ -1712,7 +1760,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1746,7 +1794,6 @@
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
@@ -1797,8 +1844,9 @@
       <c r="G16" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="I16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
@@ -1808,7 +1856,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1846,8 +1894,9 @@
         <v>54</v>
       </c>
       <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
+      <c r="I17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="J17" s="26"/>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
@@ -1857,7 +1906,7 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -1889,7 +1938,6 @@
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
       <c r="G18" s="35"/>
-      <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
       <c r="K18" s="17"/>
@@ -1938,8 +1986,9 @@
       <c r="G19" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="I19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
@@ -1949,7 +1998,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -1989,8 +2038,9 @@
       <c r="G20" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="I20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
@@ -2000,7 +2050,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2030,7 +2080,6 @@
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="21"/>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
@@ -2079,8 +2128,9 @@
       <c r="G22" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="I22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
@@ -2090,7 +2140,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2130,8 +2180,9 @@
       <c r="G23" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="I23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
@@ -2141,7 +2192,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2173,7 +2224,6 @@
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="35"/>
-      <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
@@ -2212,7 +2262,6 @@
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="26"/>
-      <c r="H25" s="21"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
       <c r="K25" s="21"/>
@@ -2260,8 +2309,9 @@
       <c r="G26" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
+      <c r="I26" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="J26" s="17"/>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
@@ -2665,13 +2715,13 @@
       <c r="AA39" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:P39 H2:P26 C2:F26">
-    <cfRule type="containsBlanks" dxfId="6" priority="2">
+  <conditionalFormatting sqref="C27:P39 C2:F26 I2:P26">
+    <cfRule type="containsBlanks" dxfId="8" priority="2">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G26">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="1">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2687,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2699,14 +2749,16 @@
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="7" width="6.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="5.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="73.140625" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="21" width="7.5703125" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" customWidth="1"/>
+    <col min="18" max="18" width="37" customWidth="1"/>
+    <col min="19" max="21" width="7.5703125" customWidth="1"/>
     <col min="22" max="23" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2759,8 +2811,12 @@
       <c r="P1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
+      <c r="Q1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
@@ -2777,27 +2833,33 @@
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="13"/>
+      <c r="E2" s="13">
+        <v>8.75</v>
+      </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="15">
         <v>9</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="15">
+        <v>9.5</v>
+      </c>
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16">
         <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
-        <v>0</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="M2" s="15">
         <f t="shared" ref="M2:M26" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
-        <v>0.9</v>
+        <v>1.85</v>
       </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
       <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
+      <c r="Q2" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -2911,7 +2973,9 @@
       <c r="P5" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -2973,7 +3037,9 @@
       <c r="H7" s="23">
         <v>10</v>
       </c>
-      <c r="I7" s="23"/>
+      <c r="I7" s="23">
+        <v>10</v>
+      </c>
       <c r="J7" s="23"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16">
@@ -2982,14 +3048,16 @@
       </c>
       <c r="M7" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="25"/>
       <c r="P7" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
@@ -3052,8 +3120,12 @@
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="H9" s="15">
+        <v>8</v>
+      </c>
+      <c r="I9" s="15">
+        <v>10</v>
+      </c>
       <c r="J9" s="15"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16">
@@ -3062,7 +3134,7 @@
       </c>
       <c r="M9" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -3129,7 +3201,9 @@
       <c r="H11" s="15">
         <v>10</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="15">
+        <v>10</v>
+      </c>
       <c r="J11" s="15"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16">
@@ -3138,14 +3212,16 @@
       </c>
       <c r="M11" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="18"/>
       <c r="O11" s="25"/>
       <c r="P11" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -3199,22 +3275,26 @@
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="22"/>
+      <c r="E13" s="22">
+        <v>9</v>
+      </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="23">
         <v>9.5</v>
       </c>
-      <c r="I13" s="23"/>
+      <c r="I13" s="23">
+        <v>10</v>
+      </c>
       <c r="J13" s="23"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="2"/>
-        <v>0.95</v>
+        <v>1.95</v>
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -3237,7 +3317,9 @@
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="22"/>
+      <c r="E14" s="22">
+        <v>7.25</v>
+      </c>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="15">
@@ -3248,7 +3330,7 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4166666666666665</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="2"/>
@@ -3259,7 +3341,9 @@
       <c r="P14" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q14" s="10"/>
+      <c r="Q14" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
@@ -3321,7 +3405,9 @@
       <c r="H16" s="15">
         <v>6</v>
       </c>
-      <c r="I16" s="15"/>
+      <c r="I16" s="15">
+        <v>9.5</v>
+      </c>
       <c r="J16" s="15"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16">
@@ -3330,7 +3416,7 @@
       </c>
       <c r="M16" s="15">
         <f t="shared" si="2"/>
-        <v>0.6</v>
+        <v>1.5499999999999998</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="25"/>
@@ -3361,7 +3447,9 @@
       <c r="H17" s="23">
         <v>9</v>
       </c>
-      <c r="I17" s="23"/>
+      <c r="I17" s="23">
+        <v>8</v>
+      </c>
       <c r="J17" s="23"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16">
@@ -3370,7 +3458,7 @@
       </c>
       <c r="M17" s="15">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -3439,7 +3527,9 @@
       <c r="H19" s="15">
         <v>10</v>
       </c>
-      <c r="I19" s="15"/>
+      <c r="I19" s="15">
+        <v>10</v>
+      </c>
       <c r="J19" s="15"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16">
@@ -3448,14 +3538,16 @@
       </c>
       <c r="M19" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
       <c r="P19" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q19" s="10"/>
+      <c r="Q19" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -3481,7 +3573,9 @@
       <c r="H20" s="15">
         <v>9</v>
       </c>
-      <c r="I20" s="15"/>
+      <c r="I20" s="15">
+        <v>10</v>
+      </c>
       <c r="J20" s="15"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16">
@@ -3490,7 +3584,7 @@
       </c>
       <c r="M20" s="15">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -3551,22 +3645,26 @@
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="22"/>
+      <c r="E22" s="22">
+        <v>7.5</v>
+      </c>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="23">
         <v>9</v>
       </c>
-      <c r="I22" s="23"/>
+      <c r="I22" s="23">
+        <v>10</v>
+      </c>
       <c r="J22" s="23"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="M22" s="15">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1.9</v>
       </c>
       <c r="N22" s="18"/>
       <c r="O22" s="25"/>
@@ -3591,29 +3689,35 @@
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="22"/>
+      <c r="E23" s="22">
+        <v>8.75</v>
+      </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
       <c r="H23" s="15">
         <v>7</v>
       </c>
-      <c r="I23" s="15"/>
+      <c r="I23" s="23">
+        <v>9.5</v>
+      </c>
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.9166666666666665</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>1.65</v>
       </c>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
       <c r="P23" s="10">
         <v>0.2</v>
       </c>
-      <c r="Q23" s="10"/>
+      <c r="Q23" s="10">
+        <v>0.1</v>
+      </c>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
@@ -3702,7 +3806,9 @@
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="22"/>
+      <c r="E26" s="22">
+        <v>7.25</v>
+      </c>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="15">
@@ -3713,7 +3819,7 @@
       <c r="K26" s="16"/>
       <c r="L26" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4166666666666665</v>
       </c>
       <c r="M26" s="23">
         <f t="shared" si="2"/>
@@ -4057,7 +4163,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M39">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 08: added grades
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="93">
   <si>
     <t>Nr.</t>
   </si>
@@ -293,6 +293,12 @@
   </si>
   <si>
     <t>Builder Pattern</t>
+  </si>
+  <si>
+    <t>DP1</t>
+  </si>
+  <si>
+    <t>*max 1p la nota de pe proiect</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -517,6 +523,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,7 +797,7 @@
     <tableColumn id="15" name="Comments"/>
     <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="2"/>
     <tableColumn id="17" name="Builder Pattern" dataDxfId="1"/>
-    <tableColumn id="18" name="Column1" dataDxfId="0"/>
+    <tableColumn id="18" name="DP1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1054,7 +1069,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1167,7 +1182,9 @@
       <c r="I2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K2" s="17"/>
       <c r="L2" s="14"/>
       <c r="M2" s="17"/>
@@ -1176,7 +1193,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1307,7 +1324,9 @@
       <c r="I5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
@@ -1316,7 +1335,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1401,7 +1420,9 @@
       <c r="I7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="21"/>
+      <c r="J7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
@@ -1410,7 +1431,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1501,7 +1522,9 @@
       <c r="I9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="21"/>
+      <c r="J9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
@@ -1510,7 +1533,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1532,7 +1555,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1543,7 +1566,7 @@
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
-      <c r="G10" s="35"/>
+      <c r="G10" s="42"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
@@ -1597,7 +1620,9 @@
       <c r="I11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="21"/>
+      <c r="J11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
@@ -1606,7 +1631,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1647,7 +1672,9 @@
       <c r="I12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J12" s="17"/>
+      <c r="J12" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
@@ -1656,7 +1683,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
@@ -1699,7 +1726,9 @@
       <c r="I13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="21"/>
+      <c r="J13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
@@ -1708,7 +1737,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1751,7 +1780,9 @@
       <c r="I14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
@@ -1760,7 +1791,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1782,7 +1813,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="48" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -1847,7 +1878,9 @@
       <c r="I16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J16" s="17"/>
+      <c r="J16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
@@ -1856,7 +1889,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1897,7 +1930,9 @@
       <c r="I17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="26"/>
+      <c r="J17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="K17" s="26"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
@@ -1906,7 +1941,7 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -1989,7 +2024,9 @@
       <c r="I19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="21"/>
+      <c r="J19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -1998,7 +2035,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -2041,7 +2078,9 @@
       <c r="I20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J20" s="17"/>
+      <c r="J20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -2050,7 +2089,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2131,7 +2170,9 @@
       <c r="I22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="17"/>
+      <c r="J22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
@@ -2140,7 +2181,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2183,7 +2224,9 @@
       <c r="I23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="21"/>
+      <c r="J23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
@@ -2192,7 +2235,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2738,7 +2781,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2757,7 +2800,7 @@
     <col min="15" max="15" width="15.28515625" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="7.5703125" customWidth="1"/>
-    <col min="18" max="18" width="37" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" customWidth="1"/>
     <col min="19" max="21" width="7.5703125" customWidth="1"/>
     <col min="22" max="23" width="15.140625" customWidth="1"/>
   </cols>
@@ -2815,7 +2858,7 @@
         <v>90</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
@@ -2836,7 +2879,9 @@
       <c r="E2" s="13">
         <v>8.75</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="13">
+        <v>10</v>
+      </c>
       <c r="G2" s="13"/>
       <c r="H2" s="15">
         <v>9</v>
@@ -2848,7 +2893,7 @@
       <c r="K2" s="16"/>
       <c r="L2" s="16">
         <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
-        <v>2.9166666666666665</v>
+        <v>6.25</v>
       </c>
       <c r="M2" s="15">
         <f t="shared" ref="M2:M26" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
@@ -2877,16 +2922,18 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="22"/>
+      <c r="E3" s="22">
+        <v>1</v>
+      </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
       <c r="J3" s="23"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M3" s="15">
         <f t="shared" si="2"/>
@@ -2952,21 +2999,25 @@
       <c r="E5" s="22">
         <v>9.5</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="22">
+        <v>9.75</v>
+      </c>
       <c r="G5" s="22"/>
       <c r="H5" s="23">
         <v>10</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="23">
+        <v>10</v>
+      </c>
       <c r="J5" s="23"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16">
         <f t="shared" si="1"/>
-        <v>3.1666666666666665</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="M5" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" s="24"/>
       <c r="O5" s="25"/>
@@ -3032,7 +3083,9 @@
       <c r="E7" s="22">
         <v>10</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="22">
+        <v>10</v>
+      </c>
       <c r="G7" s="22"/>
       <c r="H7" s="23">
         <v>10</v>
@@ -3044,7 +3097,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" si="2"/>
@@ -3075,18 +3128,20 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="22"/>
+      <c r="E8" s="22">
+        <v>5</v>
+      </c>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23">
         <v>10</v>
       </c>
-      <c r="I8" s="23"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="23"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="2"/>
@@ -3152,21 +3207,23 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="47" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="46">
+        <v>1</v>
+      </c>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="15"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="2"/>
@@ -3222,7 +3279,9 @@
       <c r="Q11" s="10">
         <v>0.1</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="10">
+        <v>0.08</v>
+      </c>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
@@ -3239,16 +3298,18 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="22"/>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="2"/>
@@ -3278,7 +3339,9 @@
       <c r="E13" s="22">
         <v>9</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="22">
+        <v>9.75</v>
+      </c>
       <c r="G13" s="22"/>
       <c r="H13" s="23">
         <v>9.5</v>
@@ -3290,7 +3353,7 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6.25</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="2"/>
@@ -3325,7 +3388,9 @@
       <c r="H14" s="15">
         <v>8</v>
       </c>
-      <c r="I14" s="15"/>
+      <c r="I14" s="15">
+        <v>9</v>
+      </c>
       <c r="J14" s="15"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16">
@@ -3334,7 +3399,7 @@
       </c>
       <c r="M14" s="15">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="N14" s="18"/>
       <c r="O14" s="25"/>
@@ -3356,21 +3421,23 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="48" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="22"/>
+      <c r="E15" s="46">
+        <v>1</v>
+      </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="23"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M15" s="15">
         <f t="shared" si="2"/>
@@ -3400,7 +3467,9 @@
       <c r="E16" s="22">
         <v>8.5</v>
       </c>
-      <c r="F16" s="22"/>
+      <c r="F16" s="22">
+        <v>10</v>
+      </c>
       <c r="G16" s="22"/>
       <c r="H16" s="15">
         <v>6</v>
@@ -3412,7 +3481,7 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
-        <v>2.8333333333333335</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="2"/>
@@ -3424,7 +3493,9 @@
         <v>0.2</v>
       </c>
       <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
+      <c r="R16" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
@@ -3441,7 +3512,9 @@
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="22"/>
+      <c r="E17" s="22">
+        <v>5</v>
+      </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
       <c r="H17" s="23">
@@ -3454,7 +3527,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="2"/>
@@ -3522,7 +3595,9 @@
       <c r="E19" s="22">
         <v>10</v>
       </c>
-      <c r="F19" s="22"/>
+      <c r="F19" s="22">
+        <v>9.5</v>
+      </c>
       <c r="G19" s="22"/>
       <c r="H19" s="15">
         <v>10</v>
@@ -3534,7 +3609,7 @@
       <c r="K19" s="16"/>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>6.5</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="2"/>
@@ -3548,7 +3623,9 @@
       <c r="Q19" s="10">
         <v>0.1</v>
       </c>
-      <c r="R19" s="10"/>
+      <c r="R19" s="10">
+        <v>0.04</v>
+      </c>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
@@ -3592,7 +3669,9 @@
         <v>0.2</v>
       </c>
       <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
+      <c r="R20" s="10">
+        <v>0.04</v>
+      </c>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
@@ -3648,7 +3727,9 @@
       <c r="E22" s="22">
         <v>7.5</v>
       </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="22">
+        <v>9.5</v>
+      </c>
       <c r="G22" s="22"/>
       <c r="H22" s="23">
         <v>9</v>
@@ -3660,7 +3741,7 @@
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="M22" s="15">
         <f t="shared" si="2"/>
@@ -3718,7 +3799,9 @@
       <c r="Q23" s="10">
         <v>0.1</v>
       </c>
-      <c r="R23" s="10"/>
+      <c r="R23" s="10">
+        <v>0.1</v>
+      </c>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
@@ -3814,7 +3897,7 @@
       <c r="H26" s="15">
         <v>9</v>
       </c>
-      <c r="I26" s="15"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="15"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16">
@@ -3902,7 +3985,9 @@
       <c r="M29" s="15"/>
       <c r="N29" s="18"/>
       <c r="O29" s="18"/>
-      <c r="P29" s="10"/>
+      <c r="P29" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
@@ -4168,8 +4253,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lab 09: added grades.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
   <si>
     <t>Nr.</t>
   </si>
@@ -342,7 +342,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +373,18 @@
         <bgColor rgb="FFD7D7D7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -401,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -524,14 +536,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,7 +1082,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1185,7 +1198,9 @@
       <c r="J2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="17"/>
+      <c r="K2" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="L2" s="14"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -1193,7 +1208,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1211,11 +1226,11 @@
       <c r="AA2" s="10"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="19">
+      <c r="A3" s="48">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="47" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -1327,7 +1342,9 @@
       <c r="J5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="21"/>
+      <c r="K5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
@@ -1335,7 +1352,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1423,7 +1440,9 @@
       <c r="J7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="21"/>
+      <c r="K7" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
@@ -1431,7 +1450,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1473,7 +1492,9 @@
         <v>54</v>
       </c>
       <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="K8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
@@ -1481,7 +1502,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1525,7 +1546,9 @@
       <c r="J9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="21"/>
+      <c r="K9" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
@@ -1533,7 +1556,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1555,7 +1578,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="46" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1675,7 +1698,9 @@
       <c r="J12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K12" s="17"/>
+      <c r="K12" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
@@ -1683,7 +1708,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
@@ -1729,7 +1754,9 @@
       <c r="J13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="21"/>
+      <c r="K13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -1737,7 +1764,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1783,7 +1810,9 @@
       <c r="J14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="17"/>
+      <c r="K14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -1791,7 +1820,7 @@
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1813,7 +1842,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="26" t="s">
@@ -1881,7 +1910,9 @@
       <c r="J16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="17"/>
+      <c r="K16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
@@ -1889,7 +1920,7 @@
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -1933,7 +1964,9 @@
       <c r="J17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="26"/>
+      <c r="K17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
@@ -1941,7 +1974,7 @@
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -2027,7 +2060,9 @@
       <c r="J19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K19" s="21"/>
+      <c r="K19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -2035,7 +2070,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -2081,7 +2116,9 @@
       <c r="J20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K20" s="17"/>
+      <c r="K20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
@@ -2089,7 +2126,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2173,7 +2210,9 @@
       <c r="J22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="17"/>
+      <c r="K22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -2181,7 +2220,7 @@
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2227,7 +2266,9 @@
       <c r="J23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="21"/>
+      <c r="K23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
@@ -2235,7 +2276,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2356,7 +2397,9 @@
         <v>54</v>
       </c>
       <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
+      <c r="K26" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -2781,7 +2824,7 @@
   <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2793,7 +2836,7 @@
     <col min="5" max="7" width="6.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="14" width="18.7109375" customWidth="1"/>
@@ -2917,7 +2960,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="47" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="11"/>
@@ -2925,19 +2968,31 @@
       <c r="E3" s="22">
         <v>1</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="16"/>
+      <c r="F3" s="49">
+        <v>1</v>
+      </c>
+      <c r="G3" s="22">
+        <v>1</v>
+      </c>
+      <c r="H3" s="49">
+        <v>1</v>
+      </c>
+      <c r="I3" s="49">
+        <v>1</v>
+      </c>
+      <c r="J3" s="23">
+        <v>1</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1</v>
+      </c>
       <c r="L3" s="16">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M3" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
@@ -3093,7 +3148,9 @@
       <c r="I7" s="23">
         <v>10</v>
       </c>
-      <c r="J7" s="23"/>
+      <c r="J7" s="23">
+        <v>10</v>
+      </c>
       <c r="K7" s="16"/>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
@@ -3101,7 +3158,7 @@
       </c>
       <c r="M7" s="15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="25"/>
@@ -3136,7 +3193,9 @@
       <c r="H8" s="23">
         <v>10</v>
       </c>
-      <c r="I8" s="46"/>
+      <c r="I8" s="49">
+        <v>8</v>
+      </c>
       <c r="J8" s="23"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16">
@@ -3145,7 +3204,7 @@
       </c>
       <c r="M8" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="N8" s="24"/>
       <c r="O8" s="25"/>
@@ -3173,7 +3232,9 @@
       <c r="E9" s="22">
         <v>9.5</v>
       </c>
-      <c r="F9" s="22"/>
+      <c r="F9" s="22">
+        <v>8</v>
+      </c>
       <c r="G9" s="22"/>
       <c r="H9" s="15">
         <v>8</v>
@@ -3185,7 +3246,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
-        <v>3.1666666666666665</v>
+        <v>5.833333333333333</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="2"/>
@@ -3207,27 +3268,39 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="46" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="46">
+      <c r="E10" s="49">
         <v>1</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="16"/>
+      <c r="F10" s="22">
+        <v>1</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49">
+        <v>1</v>
+      </c>
+      <c r="I10" s="49">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15">
+        <v>1</v>
+      </c>
+      <c r="K10" s="16">
+        <v>1</v>
+      </c>
       <c r="L10" s="16">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
@@ -3303,8 +3376,12 @@
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="H12" s="49">
+        <v>5</v>
+      </c>
+      <c r="I12" s="49">
+        <v>7</v>
+      </c>
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16">
@@ -3313,7 +3390,7 @@
       </c>
       <c r="M12" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -3383,7 +3460,9 @@
       <c r="E14" s="22">
         <v>7.25</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="22">
+        <v>9</v>
+      </c>
       <c r="G14" s="22"/>
       <c r="H14" s="15">
         <v>8</v>
@@ -3395,7 +3474,7 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
-        <v>2.4166666666666665</v>
+        <v>5.416666666666667</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="2"/>
@@ -3421,27 +3500,39 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="46">
+      <c r="E15" s="49">
         <v>1</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="16"/>
+      <c r="F15" s="22">
+        <v>1</v>
+      </c>
+      <c r="G15" s="22">
+        <v>1</v>
+      </c>
+      <c r="H15" s="49">
+        <v>1</v>
+      </c>
+      <c r="I15" s="49">
+        <v>1</v>
+      </c>
+      <c r="J15" s="23">
+        <v>1</v>
+      </c>
+      <c r="K15" s="16">
+        <v>1</v>
+      </c>
       <c r="L15" s="16">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="M15" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="25"/>
@@ -3515,7 +3606,9 @@
       <c r="E17" s="22">
         <v>5</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="22">
+        <v>6.5</v>
+      </c>
       <c r="G17" s="22"/>
       <c r="H17" s="23">
         <v>9</v>
@@ -3527,7 +3620,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16">
         <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
+        <v>3.8333333333333335</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="2"/>
@@ -3645,7 +3738,9 @@
       <c r="E20" s="22">
         <v>8.5</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="22">
+        <v>9.5</v>
+      </c>
       <c r="G20" s="22"/>
       <c r="H20" s="15">
         <v>9</v>
@@ -3657,7 +3752,7 @@
       <c r="K20" s="16"/>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
-        <v>2.8333333333333335</v>
+        <v>6</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" si="2"/>
@@ -3773,7 +3868,9 @@
       <c r="E23" s="22">
         <v>8.75</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="22">
+        <v>10</v>
+      </c>
       <c r="G23" s="22"/>
       <c r="H23" s="15">
         <v>7</v>
@@ -3785,7 +3882,7 @@
       <c r="K23" s="16"/>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
-        <v>2.9166666666666665</v>
+        <v>6.25</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="2"/>
@@ -3897,7 +3994,9 @@
       <c r="H26" s="15">
         <v>9</v>
       </c>
-      <c r="I26" s="46"/>
+      <c r="I26" s="49">
+        <v>7</v>
+      </c>
       <c r="J26" s="15"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16">
@@ -3906,7 +4005,7 @@
       </c>
       <c r="M26" s="23">
         <f t="shared" si="2"/>
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>

</xml_diff>

<commit_message>
Lab 10: added exercise. added grading for documentation PD3.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="101">
   <si>
     <t>Nr.</t>
   </si>
@@ -299,6 +299,30 @@
   </si>
   <si>
     <t>*max 1p la nota de pe proiect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      P</t>
+  </si>
+  <si>
+    <t>Present lab activity at laboratory session</t>
+  </si>
+  <si>
+    <t>Send lab activity per email</t>
+  </si>
+  <si>
+    <t>RECUPERARE LAB</t>
+  </si>
+  <si>
+    <t>RECUPERAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab activity was received and accepted </t>
+  </si>
+  <si>
+    <t>Will be presented in RESTANTE</t>
+  </si>
+  <si>
+    <t>MAX 1 DP /+ 1A</t>
   </si>
 </sst>
 </file>
@@ -342,7 +366,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +409,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -413,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -546,64 +588,60 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -669,25 +707,57 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -740,14 +810,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="firstRowStripe" dxfId="13"/>
-      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -782,16 +852,16 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="6"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="5"/>
-    <tableColumn id="21" name="Column1" dataDxfId="4"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="10"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="9"/>
+    <tableColumn id="21" name="Column1" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:R39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:R40">
   <tableColumns count="18">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
@@ -808,9 +878,9 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="2"/>
-    <tableColumn id="17" name="Builder Pattern" dataDxfId="1"/>
-    <tableColumn id="18" name="DP1" dataDxfId="0"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="7"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="6"/>
+    <tableColumn id="18" name="DP1" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1079,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA39"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44:T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1093,7 +1163,7 @@
     <col min="17" max="17" width="19.140625" customWidth="1"/>
     <col min="18" max="18" width="16.28515625" customWidth="1"/>
     <col min="19" max="19" width="15.85546875" customWidth="1"/>
-    <col min="20" max="20" width="25.28515625" customWidth="1"/>
+    <col min="20" max="20" width="36.7109375" customWidth="1"/>
     <col min="21" max="21" width="24" customWidth="1"/>
     <col min="22" max="27" width="7.5703125" customWidth="1"/>
   </cols>
@@ -1487,11 +1557,11 @@
       <c r="F8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="52"/>
       <c r="I8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="17" t="s">
         <v>54</v>
       </c>
@@ -1536,7 +1606,7 @@
       <c r="E9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="26" t="s">
         <v>54</v>
       </c>
@@ -1646,7 +1716,7 @@
       <c r="J11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="21"/>
+      <c r="K11" s="52"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -1688,9 +1758,9 @@
       <c r="E12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="35" t="s">
-        <v>54</v>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52" t="s">
+        <v>93</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>54</v>
@@ -1957,7 +2027,7 @@
       <c r="F17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="26"/>
+      <c r="G17" s="52"/>
       <c r="I17" s="26" t="s">
         <v>54</v>
       </c>
@@ -2396,7 +2466,7 @@
       <c r="I26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="17"/>
+      <c r="J26" s="52"/>
       <c r="K26" s="17" t="s">
         <v>54</v>
       </c>
@@ -2800,14 +2870,35 @@
       <c r="Z39" s="10"/>
       <c r="AA39" s="10"/>
     </row>
+    <row r="41" spans="1:27" ht="15" customHeight="1">
+      <c r="S41" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="T41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" ht="15" customHeight="1">
+      <c r="T42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" ht="15" customHeight="1">
+      <c r="S43" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="T43" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:P39 C2:F26 I2:P26">
-    <cfRule type="containsBlanks" dxfId="8" priority="2">
+  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I12:P25 I11:J11 L11:P11 I26 K26:P26">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+  <conditionalFormatting sqref="G2:G7 G9:G11 G13:G16 G18:G26">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2821,10 +2912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -3188,7 +3279,7 @@
       <c r="E8" s="22">
         <v>5</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23">
         <v>10</v>
@@ -3326,7 +3417,7 @@
       <c r="E11" s="22">
         <v>10</v>
       </c>
-      <c r="F11" s="22"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="22"/>
       <c r="H11" s="15">
         <v>10</v>
@@ -3371,10 +3462,10 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="22">
+      <c r="E12" s="51">
         <v>1</v>
       </c>
-      <c r="F12" s="22"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="22"/>
       <c r="H12" s="49">
         <v>5</v>
@@ -3989,7 +4080,7 @@
       <c r="E26" s="22">
         <v>7.25</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="50"/>
       <c r="G26" s="22"/>
       <c r="H26" s="15">
         <v>9</v>
@@ -4345,9 +4436,17 @@
       <c r="V39" s="10"/>
       <c r="W39" s="10"/>
     </row>
+    <row r="40" spans="1:23" ht="15" customHeight="1">
+      <c r="P40" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L2:M39">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="L2:M40">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 11: added exercise. added grading.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="102">
   <si>
     <t>Nr.</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>MAX 1 DP /+ 1A</t>
+  </si>
+  <si>
+    <t>DP2</t>
   </si>
 </sst>
 </file>
@@ -588,105 +591,20 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <b val="0"/>
@@ -762,6 +680,90 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFE7F9EF"/>
           <bgColor rgb="FFE7F9EF"/>
         </patternFill>
@@ -810,14 +812,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -852,17 +854,17 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="10"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="9"/>
-    <tableColumn id="21" name="Column1" dataDxfId="8"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="7"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="6"/>
+    <tableColumn id="21" name="Column1" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:R40">
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:S40">
+  <tableColumns count="19">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
     <tableColumn id="3" name="H1"/>
@@ -878,9 +880,10 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="7"/>
-    <tableColumn id="17" name="Builder Pattern" dataDxfId="6"/>
-    <tableColumn id="18" name="DP1" dataDxfId="5"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="3"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="2"/>
+    <tableColumn id="18" name="DP1" dataDxfId="1"/>
+    <tableColumn id="19" name="DP2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44:T44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1271,14 +1274,16 @@
       <c r="K2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1415,14 +1420,16 @@
       <c r="K5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="21"/>
+      <c r="L5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1513,14 +1520,16 @@
       <c r="K7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="21"/>
+      <c r="L7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1557,22 +1566,24 @@
       <c r="F8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="52"/>
+      <c r="G8" s="51"/>
       <c r="I8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="52"/>
+      <c r="J8" s="51"/>
       <c r="K8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="17"/>
+      <c r="L8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1606,7 +1617,7 @@
       <c r="E9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="52"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="26" t="s">
         <v>54</v>
       </c>
@@ -1619,14 +1630,16 @@
       <c r="K9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="21"/>
+      <c r="L9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1716,15 +1729,17 @@
       <c r="J11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="52"/>
-      <c r="L11" s="21"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1758,8 +1773,8 @@
       <c r="E12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52" t="s">
+      <c r="F12" s="51"/>
+      <c r="G12" s="51" t="s">
         <v>93</v>
       </c>
       <c r="I12" s="17" t="s">
@@ -1771,7 +1786,7 @@
       <c r="K12" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="17"/>
+      <c r="L12" s="51"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
@@ -1827,14 +1842,16 @@
       <c r="K13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="21"/>
+      <c r="L13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1883,14 +1900,16 @@
       <c r="K14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="17"/>
+      <c r="L14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1983,14 +2002,16 @@
       <c r="K16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L16" s="17"/>
+      <c r="L16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -2027,7 +2048,7 @@
       <c r="F17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="52"/>
+      <c r="G17" s="51"/>
       <c r="I17" s="26" t="s">
         <v>54</v>
       </c>
@@ -2037,14 +2058,16 @@
       <c r="K17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="26"/>
+      <c r="L17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -2133,14 +2156,16 @@
       <c r="K19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="21"/>
+      <c r="L19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -2189,14 +2214,16 @@
       <c r="K20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="17"/>
+      <c r="L20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2283,14 +2310,16 @@
       <c r="K22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L22" s="17"/>
+      <c r="L22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2339,14 +2368,16 @@
       <c r="K23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L23" s="21"/>
+      <c r="L23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2466,11 +2497,13 @@
       <c r="I26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="52"/>
+      <c r="J26" s="51"/>
       <c r="K26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L26" s="17"/>
+      <c r="L26" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
@@ -2871,7 +2904,7 @@
       <c r="AA39" s="10"/>
     </row>
     <row r="41" spans="1:27" ht="15" customHeight="1">
-      <c r="S41" s="52" t="s">
+      <c r="S41" s="51" t="s">
         <v>96</v>
       </c>
       <c r="T41" t="s">
@@ -2884,7 +2917,7 @@
       </c>
     </row>
     <row r="43" spans="1:27" ht="15" customHeight="1">
-      <c r="S43" s="53" t="s">
+      <c r="S43" s="52" t="s">
         <v>97</v>
       </c>
       <c r="T43" t="s">
@@ -2892,13 +2925,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I12:P25 I11:J11 L11:P11 I26 K26:P26">
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
+  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:P26 I12:K12 M12:P12">
+    <cfRule type="containsBlanks" dxfId="9" priority="3">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7 G9:G11 G13:G16 G18:G26">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="8" priority="2">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2915,7 +2948,7 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2994,7 +3027,9 @@
       <c r="R1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="9"/>
+      <c r="S1" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
@@ -3023,7 +3058,7 @@
       <c r="I2" s="15">
         <v>9.5</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="54"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16">
         <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
@@ -3040,7 +3075,9 @@
         <v>0.1</v>
       </c>
       <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="S2" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
@@ -3155,7 +3192,7 @@
       <c r="I5" s="23">
         <v>10</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="54"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16">
         <f t="shared" si="1"/>
@@ -3174,7 +3211,9 @@
         <v>0.1</v>
       </c>
       <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
+      <c r="S5" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
@@ -3260,7 +3299,9 @@
         <v>0.1</v>
       </c>
       <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
+      <c r="S7" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
@@ -3279,7 +3320,9 @@
       <c r="E8" s="22">
         <v>5</v>
       </c>
-      <c r="F8" s="50"/>
+      <c r="F8" s="50">
+        <v>1</v>
+      </c>
       <c r="G8" s="22"/>
       <c r="H8" s="23">
         <v>10</v>
@@ -3287,11 +3330,11 @@
       <c r="I8" s="49">
         <v>8</v>
       </c>
-      <c r="J8" s="23"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16">
         <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="2"/>
@@ -3333,7 +3376,7 @@
       <c r="I9" s="15">
         <v>10</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
@@ -3348,7 +3391,9 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
+      <c r="S9" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
@@ -3417,7 +3462,9 @@
       <c r="E11" s="22">
         <v>10</v>
       </c>
-      <c r="F11" s="50"/>
+      <c r="F11" s="49">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="G11" s="22"/>
       <c r="H11" s="15">
         <v>10</v>
@@ -3425,15 +3472,17 @@
       <c r="I11" s="15">
         <v>10</v>
       </c>
-      <c r="J11" s="15"/>
+      <c r="J11" s="15">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K11" s="16"/>
       <c r="L11" s="16">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335</v>
+        <v>6.1000000000000005</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.92</v>
       </c>
       <c r="N11" s="18"/>
       <c r="O11" s="25"/>
@@ -3446,7 +3495,9 @@
       <c r="R11" s="10">
         <v>0.08</v>
       </c>
-      <c r="S11" s="10"/>
+      <c r="S11" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -3462,10 +3513,12 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="51">
+      <c r="E12" s="50">
         <v>1</v>
       </c>
-      <c r="F12" s="50"/>
+      <c r="F12" s="50">
+        <v>1</v>
+      </c>
       <c r="G12" s="22"/>
       <c r="H12" s="49">
         <v>5</v>
@@ -3473,11 +3526,11 @@
       <c r="I12" s="49">
         <v>7</v>
       </c>
-      <c r="J12" s="15"/>
+      <c r="J12" s="54"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="2"/>
@@ -3488,7 +3541,9 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
+      <c r="S12" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
@@ -3517,7 +3572,7 @@
       <c r="I13" s="23">
         <v>10</v>
       </c>
-      <c r="J13" s="23"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
@@ -3561,7 +3616,7 @@
       <c r="I14" s="15">
         <v>9</v>
       </c>
-      <c r="J14" s="15"/>
+      <c r="J14" s="54"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
@@ -3580,7 +3635,9 @@
         <v>0.1</v>
       </c>
       <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
+      <c r="S14" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
@@ -3659,7 +3716,7 @@
       <c r="I16" s="15">
         <v>9.5</v>
       </c>
-      <c r="J16" s="15"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
@@ -3678,7 +3735,9 @@
       <c r="R16" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S16" s="10"/>
+      <c r="S16" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
@@ -3707,7 +3766,9 @@
       <c r="I17" s="23">
         <v>8</v>
       </c>
-      <c r="J17" s="23"/>
+      <c r="J17" s="23">
+        <v>6</v>
+      </c>
       <c r="K17" s="16"/>
       <c r="L17" s="16">
         <f t="shared" si="1"/>
@@ -3715,7 +3776,7 @@
       </c>
       <c r="M17" s="15">
         <f t="shared" si="2"/>
-        <v>1.7000000000000002</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -3789,7 +3850,9 @@
       <c r="I19" s="15">
         <v>10</v>
       </c>
-      <c r="J19" s="15"/>
+      <c r="J19" s="15">
+        <v>9</v>
+      </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
@@ -3797,7 +3860,7 @@
       </c>
       <c r="M19" s="15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.9</v>
       </c>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -3839,7 +3902,9 @@
       <c r="I20" s="15">
         <v>10</v>
       </c>
-      <c r="J20" s="15"/>
+      <c r="J20" s="15">
+        <v>6</v>
+      </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
@@ -3847,7 +3912,7 @@
       </c>
       <c r="M20" s="15">
         <f t="shared" si="2"/>
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -3923,7 +3988,7 @@
       <c r="I22" s="23">
         <v>10</v>
       </c>
-      <c r="J22" s="23"/>
+      <c r="J22" s="54"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
@@ -3969,7 +4034,9 @@
       <c r="I23" s="23">
         <v>9.5</v>
       </c>
-      <c r="J23" s="15"/>
+      <c r="J23" s="15">
+        <v>6.5</v>
+      </c>
       <c r="K23" s="16"/>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
@@ -3977,7 +4044,7 @@
       </c>
       <c r="M23" s="15">
         <f t="shared" si="2"/>
-        <v>1.65</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
@@ -3990,7 +4057,9 @@
       <c r="R23" s="10">
         <v>0.1</v>
       </c>
-      <c r="S23" s="10"/>
+      <c r="S23" s="10">
+        <v>0.1</v>
+      </c>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
@@ -4080,7 +4149,9 @@
       <c r="E26" s="22">
         <v>7.25</v>
       </c>
-      <c r="F26" s="50"/>
+      <c r="F26" s="49">
+        <v>5.5</v>
+      </c>
       <c r="G26" s="22"/>
       <c r="H26" s="15">
         <v>9</v>
@@ -4088,11 +4159,11 @@
       <c r="I26" s="49">
         <v>7</v>
       </c>
-      <c r="J26" s="15"/>
+      <c r="J26" s="54"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16">
         <f t="shared" si="1"/>
-        <v>2.4166666666666665</v>
+        <v>4.25</v>
       </c>
       <c r="M26" s="23">
         <f t="shared" si="2"/>
@@ -4437,16 +4508,17 @@
       <c r="W39" s="10"/>
     </row>
     <row r="40" spans="1:23" ht="15" customHeight="1">
-      <c r="P40" s="54" t="s">
+      <c r="P40" s="53" t="s">
         <v>100</v>
       </c>
       <c r="Q40" t="s">
         <v>99</v>
       </c>
+      <c r="S40" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M40">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 11: added grading.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="106">
   <si>
     <t>Nr.</t>
   </si>
@@ -301,9 +301,6 @@
     <t>*max 1p la nota de pe proiect</t>
   </si>
   <si>
-    <t xml:space="preserve">      P</t>
-  </si>
-  <si>
     <t>Present lab activity at laboratory session</t>
   </si>
   <si>
@@ -329,13 +326,25 @@
   </si>
   <si>
     <t>DP3</t>
+  </si>
+  <si>
+    <t>Paste</t>
+  </si>
+  <si>
+    <t>DP4</t>
+  </si>
+  <si>
+    <t>DP5</t>
+  </si>
+  <si>
+    <t>Bonus Proiect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,8 +380,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +448,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD7D7D7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -461,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -603,11 +624,167 @@
     <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -701,90 +878,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFE7F9EF"/>
           <bgColor rgb="FFE7F9EF"/>
         </patternFill>
@@ -833,14 +926,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="secondRowStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -875,17 +968,17 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="8"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="7"/>
-    <tableColumn id="21" name="Column1" dataDxfId="6"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="14"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="13"/>
+    <tableColumn id="21" name="Column1" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:T40">
-  <tableColumns count="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:W40">
+  <tableColumns count="23">
     <tableColumn id="1" name="Nr."/>
     <tableColumn id="2" name="Nume si prenume"/>
     <tableColumn id="3" name="H1"/>
@@ -901,11 +994,14 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="4"/>
-    <tableColumn id="17" name="Builder Pattern" dataDxfId="3"/>
-    <tableColumn id="18" name="DP1" dataDxfId="2"/>
-    <tableColumn id="19" name="DP2" dataDxfId="1"/>
-    <tableColumn id="20" name="DP3" dataDxfId="0"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="11"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="10"/>
+    <tableColumn id="18" name="DP1" dataDxfId="9"/>
+    <tableColumn id="19" name="DP2" dataDxfId="8"/>
+    <tableColumn id="20" name="DP3" dataDxfId="7"/>
+    <tableColumn id="21" name="DP4" dataDxfId="2"/>
+    <tableColumn id="22" name="DP5" dataDxfId="1"/>
+    <tableColumn id="23" name="Bonus Proiect" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1177,7 +1273,7 @@
   <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1299,13 +1395,15 @@
       <c r="L2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="M2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
+      <c r="P2" s="56"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1350,7 +1448,7 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
       <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="P3" s="57"/>
       <c r="Q3" s="17">
         <f t="shared" ref="Q3:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
         <v>4</v>
@@ -1390,7 +1488,7 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
+      <c r="P4" s="56"/>
       <c r="Q4" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1445,13 +1543,15 @@
       <c r="L5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N5" s="21"/>
       <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1490,7 +1590,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
+      <c r="P6" s="56"/>
       <c r="Q6" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1545,13 +1645,15 @@
       <c r="L7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N7" s="21"/>
       <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
+      <c r="P7" s="57"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1588,24 +1690,26 @@
       <c r="F8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="51"/>
+      <c r="G8" s="55"/>
       <c r="I8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
       <c r="K8" s="17" t="s">
         <v>54</v>
       </c>
       <c r="L8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
+      <c r="P8" s="56"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1655,13 +1759,15 @@
       <c r="L9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
+      <c r="P9" s="57"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1702,7 +1808,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
+      <c r="P10" s="56"/>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -1751,17 +1857,19 @@
       <c r="J11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="51"/>
+      <c r="K11" s="52"/>
       <c r="L11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M11" s="21"/>
+      <c r="M11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
+      <c r="P11" s="57"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1783,7 +1891,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="46" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1796,8 +1904,8 @@
         <v>54</v>
       </c>
       <c r="F12" s="51"/>
-      <c r="G12" s="51" t="s">
-        <v>93</v>
+      <c r="G12" s="52" t="s">
+        <v>102</v>
       </c>
       <c r="I12" s="17" t="s">
         <v>54</v>
@@ -1809,10 +1917,10 @@
         <v>54</v>
       </c>
       <c r="L12" s="51"/>
-      <c r="M12" s="17"/>
+      <c r="M12" s="51"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
+      <c r="P12" s="56"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1867,13 +1975,15 @@
       <c r="L13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="21"/>
+      <c r="M13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N13" s="21"/>
       <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -1925,13 +2035,15 @@
       <c r="L14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="17"/>
+      <c r="M14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
+      <c r="P14" s="56"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -1972,7 +2084,7 @@
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
       <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
+      <c r="P15" s="57"/>
       <c r="Q15" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
@@ -2027,13 +2139,15 @@
       <c r="L16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="17"/>
+      <c r="M16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
+      <c r="P16" s="56"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -2083,13 +2197,15 @@
       <c r="L17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="M17" s="26"/>
+      <c r="M17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="P17" s="57"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -2128,7 +2244,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
+      <c r="P18" s="56"/>
       <c r="Q18" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2181,13 +2297,15 @@
       <c r="L19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N19" s="21"/>
       <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
+      <c r="P19" s="57"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -2239,13 +2357,15 @@
       <c r="L20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="17"/>
+      <c r="M20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
-      <c r="P20" s="17"/>
+      <c r="P20" s="56"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2282,7 +2402,7 @@
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
       <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
+      <c r="P21" s="57"/>
       <c r="Q21" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2335,13 +2455,15 @@
       <c r="L22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M22" s="17"/>
+      <c r="M22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
+      <c r="P22" s="56"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2393,13 +2515,15 @@
       <c r="L23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="21"/>
+      <c r="M23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
-      <c r="P23" s="21"/>
+      <c r="P23" s="57"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2438,7 +2562,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="P24" s="56"/>
       <c r="Q24" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2476,7 +2600,7 @@
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
       <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
+      <c r="P25" s="57"/>
       <c r="Q25" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2526,10 +2650,10 @@
       <c r="L26" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M26" s="17"/>
+      <c r="M26" s="51"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
+      <c r="P26" s="56"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
       <c r="S26" s="10" t="s">
@@ -2927,33 +3051,33 @@
     </row>
     <row r="41" spans="1:27" ht="15" customHeight="1">
       <c r="S41" s="51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="15" customHeight="1">
       <c r="T42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="15" customHeight="1">
       <c r="S43" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="T43" t="s">
         <v>97</v>
       </c>
-      <c r="T43" t="s">
-        <v>98</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:P26 I12:K12 M12:P12">
-    <cfRule type="containsBlanks" dxfId="10" priority="3">
+  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:L26 I12:K12 N12:P12 N26:P26">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7 G9:G11 G13:G16 G18:G26">
-    <cfRule type="containsBlanks" dxfId="9" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2970,7 +3094,7 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -2990,8 +3114,10 @@
     <col min="16" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="7.5703125" customWidth="1"/>
     <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="21" width="7.5703125" customWidth="1"/>
-    <col min="22" max="23" width="15.140625" customWidth="1"/>
+    <col min="19" max="20" width="7.5703125" customWidth="1"/>
+    <col min="21" max="21" width="6.28515625" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="36" customHeight="1">
@@ -3050,14 +3176,20 @@
         <v>91</v>
       </c>
       <c r="S1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="U1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11">
@@ -3082,7 +3214,9 @@
       <c r="I2" s="15">
         <v>9.5</v>
       </c>
-      <c r="J2" s="54"/>
+      <c r="J2" s="54">
+        <v>6</v>
+      </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16">
         <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
@@ -3090,7 +3224,7 @@
       </c>
       <c r="M2" s="15">
         <f t="shared" ref="M2:M26" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
-        <v>1.85</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
@@ -3102,7 +3236,9 @@
       <c r="S2" s="10">
         <v>0.1</v>
       </c>
-      <c r="T2" s="10"/>
+      <c r="T2" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
@@ -3216,7 +3352,9 @@
       <c r="I5" s="23">
         <v>10</v>
       </c>
-      <c r="J5" s="54"/>
+      <c r="J5" s="54">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="K5" s="16"/>
       <c r="L5" s="16">
         <f t="shared" si="1"/>
@@ -3224,7 +3362,7 @@
       </c>
       <c r="M5" s="15">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.83</v>
       </c>
       <c r="N5" s="24"/>
       <c r="O5" s="25"/>
@@ -3238,7 +3376,9 @@
       <c r="S5" s="10">
         <v>0.1</v>
       </c>
-      <c r="T5" s="10"/>
+      <c r="T5" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
@@ -3326,7 +3466,9 @@
       <c r="S7" s="10">
         <v>0.1</v>
       </c>
-      <c r="T7" s="10"/>
+      <c r="T7" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
@@ -3372,7 +3514,9 @@
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
+      <c r="T8" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
@@ -3400,7 +3544,9 @@
       <c r="I9" s="15">
         <v>10</v>
       </c>
-      <c r="J9" s="54"/>
+      <c r="J9" s="54">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="K9" s="16"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
@@ -3408,7 +3554,7 @@
       </c>
       <c r="M9" s="15">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2.63</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
@@ -3418,7 +3564,9 @@
       <c r="S9" s="10">
         <v>0.1</v>
       </c>
-      <c r="T9" s="10"/>
+      <c r="T9" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
@@ -3522,7 +3670,9 @@
       <c r="S11" s="10">
         <v>0.1</v>
       </c>
-      <c r="T11" s="10"/>
+      <c r="T11" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -3532,7 +3682,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="46" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="11"/>
@@ -3596,7 +3746,9 @@
       <c r="I13" s="23">
         <v>10</v>
       </c>
-      <c r="J13" s="54"/>
+      <c r="J13" s="54">
+        <v>6.5</v>
+      </c>
       <c r="K13" s="16"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
@@ -3604,7 +3756,7 @@
       </c>
       <c r="M13" s="15">
         <f t="shared" si="2"/>
-        <v>1.95</v>
+        <v>2.6</v>
       </c>
       <c r="N13" s="18"/>
       <c r="O13" s="18"/>
@@ -3612,7 +3764,9 @@
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
+      <c r="T13" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
@@ -3640,7 +3794,9 @@
       <c r="I14" s="15">
         <v>9</v>
       </c>
-      <c r="J14" s="54"/>
+      <c r="J14" s="54">
+        <v>7.5</v>
+      </c>
       <c r="K14" s="16"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
@@ -3648,7 +3804,7 @@
       </c>
       <c r="M14" s="15">
         <f t="shared" si="2"/>
-        <v>1.7000000000000002</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="N14" s="18"/>
       <c r="O14" s="25"/>
@@ -3662,7 +3818,9 @@
       <c r="S14" s="10">
         <v>0.1</v>
       </c>
-      <c r="T14" s="10"/>
+      <c r="T14" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
@@ -3703,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="M15" s="15">
-        <f t="shared" si="2"/>
+        <f>(H15/10 +I15/10 + J15/10 + K15*7/10)</f>
         <v>1</v>
       </c>
       <c r="N15" s="25"/>
@@ -3733,7 +3891,9 @@
       <c r="F16" s="22">
         <v>10</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="22">
+        <v>9.5</v>
+      </c>
       <c r="H16" s="15">
         <v>6</v>
       </c>
@@ -3744,7 +3904,7 @@
       <c r="K16" s="16"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
-        <v>6.166666666666667</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="2"/>
@@ -3762,7 +3922,9 @@
       <c r="S16" s="10">
         <v>0.1</v>
       </c>
-      <c r="T16" s="10"/>
+      <c r="T16" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
@@ -3867,7 +4029,9 @@
       <c r="F19" s="22">
         <v>9.5</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="22">
+        <v>7</v>
+      </c>
       <c r="H19" s="15">
         <v>10</v>
       </c>
@@ -3880,7 +4044,7 @@
       <c r="K19" s="16"/>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="2"/>
@@ -3919,7 +4083,9 @@
       <c r="F20" s="22">
         <v>9.5</v>
       </c>
-      <c r="G20" s="22"/>
+      <c r="G20" s="22">
+        <v>7</v>
+      </c>
       <c r="H20" s="15">
         <v>9</v>
       </c>
@@ -3932,7 +4098,7 @@
       <c r="K20" s="16"/>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="M20" s="15">
         <f t="shared" si="2"/>
@@ -4010,9 +4176,11 @@
         <v>9</v>
       </c>
       <c r="I22" s="23">
-        <v>10</v>
-      </c>
-      <c r="J22" s="54"/>
+        <v>5</v>
+      </c>
+      <c r="J22" s="54">
+        <v>6</v>
+      </c>
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
@@ -4020,7 +4188,7 @@
       </c>
       <c r="M22" s="15">
         <f t="shared" si="2"/>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="N22" s="18"/>
       <c r="O22" s="25"/>
@@ -4051,7 +4219,9 @@
       <c r="F23" s="22">
         <v>10</v>
       </c>
-      <c r="G23" s="22"/>
+      <c r="G23" s="22">
+        <v>9</v>
+      </c>
       <c r="H23" s="15">
         <v>7</v>
       </c>
@@ -4064,7 +4234,7 @@
       <c r="K23" s="16"/>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>9.25</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="2"/>
@@ -4084,7 +4254,9 @@
       <c r="S23" s="10">
         <v>0.1</v>
       </c>
-      <c r="T23" s="10"/>
+      <c r="T23" s="10">
+        <v>0.1</v>
+      </c>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
@@ -4533,17 +4705,20 @@
     </row>
     <row r="40" spans="1:23" ht="15" customHeight="1">
       <c r="P40" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M40">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 12: added grades.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="106">
   <si>
     <t>Nr.</t>
   </si>
@@ -482,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,106 +631,14 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <b val="0"/>
@@ -878,6 +786,90 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFE7F9EF"/>
           <bgColor rgb="FFE7F9EF"/>
         </patternFill>
@@ -926,14 +918,14 @@
   </dxfs>
   <tableStyles count="2">
     <tableStyle name="grades-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="20"/>
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+      <tableStyleElement type="secondRowStripe" dxfId="17"/>
     </tableStyle>
     <tableStyle name="attendance-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="secondRowStripe" dxfId="15"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -968,9 +960,9 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="14"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="13"/>
-    <tableColumn id="21" name="Column1" dataDxfId="12"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="11"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="10"/>
+    <tableColumn id="21" name="Column1" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -994,11 +986,11 @@
     <tableColumn id="13" name="Project Grade"/>
     <tableColumn id="14" name="Exam problem"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="11"/>
-    <tableColumn id="17" name="Builder Pattern" dataDxfId="10"/>
-    <tableColumn id="18" name="DP1" dataDxfId="9"/>
-    <tableColumn id="19" name="DP2" dataDxfId="8"/>
-    <tableColumn id="20" name="DP3" dataDxfId="7"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="7"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="6"/>
+    <tableColumn id="18" name="DP1" dataDxfId="5"/>
+    <tableColumn id="19" name="DP2" dataDxfId="4"/>
+    <tableColumn id="20" name="DP3" dataDxfId="3"/>
     <tableColumn id="21" name="DP4" dataDxfId="2"/>
     <tableColumn id="22" name="DP5" dataDxfId="1"/>
     <tableColumn id="23" name="Bonus Proiect" dataDxfId="0"/>
@@ -1273,7 +1265,7 @@
   <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1398,12 +1390,14 @@
       <c r="M2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O2" s="17"/>
       <c r="P2" s="56"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
@@ -1546,12 +1540,14 @@
       <c r="M5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="21"/>
+      <c r="N5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O5" s="21"/>
       <c r="P5" s="57"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
@@ -1648,12 +1644,14 @@
       <c r="M7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="21"/>
+      <c r="N7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O7" s="21"/>
       <c r="P7" s="57"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
@@ -1704,12 +1702,14 @@
       <c r="M8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="17"/>
+      <c r="N8" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O8" s="17"/>
       <c r="P8" s="56"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
@@ -1762,12 +1762,14 @@
       <c r="M9" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="21"/>
+      <c r="N9" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O9" s="21"/>
       <c r="P9" s="57"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
@@ -1864,12 +1866,14 @@
       <c r="M11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="21"/>
+      <c r="N11" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O11" s="21"/>
       <c r="P11" s="57"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
@@ -1978,12 +1982,14 @@
       <c r="M13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="21"/>
+      <c r="N13" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O13" s="21"/>
       <c r="P13" s="57"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
@@ -2038,12 +2044,14 @@
       <c r="M14" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="17"/>
+      <c r="N14" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O14" s="17"/>
       <c r="P14" s="56"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
@@ -2142,12 +2150,14 @@
       <c r="M16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N16" s="17"/>
+      <c r="N16" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O16" s="17"/>
       <c r="P16" s="56"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
@@ -2200,12 +2210,14 @@
       <c r="M17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="26"/>
+      <c r="N17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="O17" s="26"/>
       <c r="P17" s="57"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
@@ -2300,12 +2312,14 @@
       <c r="M19" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="21"/>
+      <c r="N19" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O19" s="21"/>
       <c r="P19" s="57"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
@@ -2360,12 +2374,14 @@
       <c r="M20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N20" s="17"/>
+      <c r="N20" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O20" s="17"/>
       <c r="P20" s="56"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
@@ -2458,12 +2474,14 @@
       <c r="M22" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="N22" s="17"/>
+      <c r="N22" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="O22" s="17"/>
       <c r="P22" s="56"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
@@ -2518,12 +2536,14 @@
       <c r="M23" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="21"/>
+      <c r="N23" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="O23" s="21"/>
       <c r="P23" s="57"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
@@ -2651,7 +2671,7 @@
         <v>54</v>
       </c>
       <c r="M26" s="51"/>
-      <c r="N26" s="17"/>
+      <c r="N26" s="51"/>
       <c r="O26" s="17"/>
       <c r="P26" s="56"/>
       <c r="Q26" s="17"/>
@@ -3071,13 +3091,13 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:L26 I12:K12 N12:P12 N26:P26">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+  <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:L26 I12:K12 N12:P12 O26:P26">
+    <cfRule type="containsBlanks" dxfId="13" priority="4">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7 G9:G11 G13:G16 G18:G26">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="12" priority="3">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3094,7 +3114,7 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -3207,7 +3227,9 @@
       <c r="F2" s="13">
         <v>10</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="54">
+        <v>7.7</v>
+      </c>
       <c r="H2" s="15">
         <v>9</v>
       </c>
@@ -3220,7 +3242,7 @@
       <c r="K2" s="16"/>
       <c r="L2" s="16">
         <f t="shared" ref="L2:L26" si="1">(E2 + F2 + G2)/3</f>
-        <v>6.25</v>
+        <v>8.8166666666666664</v>
       </c>
       <c r="M2" s="15">
         <f t="shared" ref="M2:M26" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
@@ -3239,11 +3261,13 @@
       <c r="T2" s="10">
         <v>0.1</v>
       </c>
-      <c r="U2" s="10"/>
+      <c r="U2" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1">
+    <row r="3" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="19">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3345,7 +3369,7 @@
       <c r="F5" s="22">
         <v>9.75</v>
       </c>
-      <c r="G5" s="22"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="23">
         <v>10</v>
       </c>
@@ -3379,7 +3403,9 @@
       <c r="T5" s="10">
         <v>0.1</v>
       </c>
-      <c r="U5" s="10"/>
+      <c r="U5" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
     </row>
@@ -3435,7 +3461,9 @@
       <c r="F7" s="22">
         <v>10</v>
       </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="54">
+        <v>7.5</v>
+      </c>
       <c r="H7" s="23">
         <v>10</v>
       </c>
@@ -3448,7 +3476,7 @@
       <c r="K7" s="16"/>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" si="2"/>
@@ -3469,7 +3497,9 @@
       <c r="T7" s="10">
         <v>0.1</v>
       </c>
-      <c r="U7" s="10"/>
+      <c r="U7" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
     </row>
@@ -3486,10 +3516,10 @@
       <c r="E8" s="22">
         <v>5</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="58">
         <v>1</v>
       </c>
-      <c r="G8" s="22"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="23">
         <v>10</v>
       </c>
@@ -3517,7 +3547,9 @@
       <c r="T8" s="10">
         <v>0.1</v>
       </c>
-      <c r="U8" s="10"/>
+      <c r="U8" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
     </row>
@@ -3537,7 +3569,9 @@
       <c r="F9" s="22">
         <v>8</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="54">
+        <v>6.5</v>
+      </c>
       <c r="H9" s="15">
         <v>8</v>
       </c>
@@ -3550,7 +3584,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
-        <v>5.833333333333333</v>
+        <v>8</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="2"/>
@@ -3567,11 +3601,13 @@
       <c r="T9" s="10">
         <v>0.1</v>
       </c>
-      <c r="U9" s="10"/>
+      <c r="U9" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1">
+    <row r="10" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A10" s="11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3637,7 +3673,9 @@
       <c r="F11" s="49">
         <v>8.3000000000000007</v>
       </c>
-      <c r="G11" s="22"/>
+      <c r="G11" s="54">
+        <v>7.2</v>
+      </c>
       <c r="H11" s="15">
         <v>10</v>
       </c>
@@ -3650,7 +3688,7 @@
       <c r="K11" s="16"/>
       <c r="L11" s="16">
         <f t="shared" si="1"/>
-        <v>6.1000000000000005</v>
+        <v>8.5</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="2"/>
@@ -3673,11 +3711,13 @@
       <c r="T11" s="10">
         <v>0.1</v>
       </c>
-      <c r="U11" s="10"/>
+      <c r="U11" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1">
+    <row r="12" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A12" s="11">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3693,22 +3733,26 @@
       <c r="F12" s="50">
         <v>1</v>
       </c>
-      <c r="G12" s="22"/>
+      <c r="G12" s="50">
+        <v>1</v>
+      </c>
       <c r="H12" s="49">
         <v>5</v>
       </c>
       <c r="I12" s="49">
         <v>7</v>
       </c>
-      <c r="J12" s="54"/>
+      <c r="J12" s="50">
+        <v>1</v>
+      </c>
       <c r="K12" s="16"/>
       <c r="L12" s="16">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="M12" s="15">
         <f t="shared" si="2"/>
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="N12" s="18"/>
       <c r="O12" s="18"/>
@@ -3739,7 +3783,9 @@
       <c r="F13" s="22">
         <v>9.75</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="54">
+        <v>9</v>
+      </c>
       <c r="H13" s="23">
         <v>9.5</v>
       </c>
@@ -3752,7 +3798,7 @@
       <c r="K13" s="16"/>
       <c r="L13" s="16">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>9.25</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="2"/>
@@ -3767,7 +3813,9 @@
       <c r="T13" s="10">
         <v>0.1</v>
       </c>
-      <c r="U13" s="10"/>
+      <c r="U13" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
     </row>
@@ -3787,7 +3835,9 @@
       <c r="F14" s="22">
         <v>9</v>
       </c>
-      <c r="G14" s="22"/>
+      <c r="G14" s="22">
+        <v>6.75</v>
+      </c>
       <c r="H14" s="15">
         <v>8</v>
       </c>
@@ -3800,7 +3850,7 @@
       <c r="K14" s="16"/>
       <c r="L14" s="16">
         <f t="shared" si="1"/>
-        <v>5.416666666666667</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="M14" s="15">
         <f t="shared" si="2"/>
@@ -3821,11 +3871,13 @@
       <c r="T14" s="10">
         <v>0.1</v>
       </c>
-      <c r="U14" s="10"/>
+      <c r="U14" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1">
+    <row r="15" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A15" s="19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3900,7 +3952,9 @@
       <c r="I16" s="15">
         <v>9.5</v>
       </c>
-      <c r="J16" s="54"/>
+      <c r="J16" s="54">
+        <v>6</v>
+      </c>
       <c r="K16" s="16"/>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
@@ -3908,7 +3962,7 @@
       </c>
       <c r="M16" s="15">
         <f t="shared" si="2"/>
-        <v>1.5499999999999998</v>
+        <v>2.15</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="25"/>
@@ -3925,7 +3979,9 @@
       <c r="T16" s="10">
         <v>0.1</v>
       </c>
-      <c r="U16" s="10"/>
+      <c r="U16" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
     </row>
@@ -3945,7 +4001,7 @@
       <c r="F17" s="22">
         <v>6.5</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="54"/>
       <c r="H17" s="23">
         <v>9</v>
       </c>
@@ -4171,7 +4227,9 @@
       <c r="F22" s="22">
         <v>9.5</v>
       </c>
-      <c r="G22" s="22"/>
+      <c r="G22" s="22">
+        <v>6</v>
+      </c>
       <c r="H22" s="23">
         <v>9</v>
       </c>
@@ -4184,7 +4242,7 @@
       <c r="K22" s="16"/>
       <c r="L22" s="16">
         <f t="shared" si="1"/>
-        <v>5.666666666666667</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="M22" s="15">
         <f t="shared" si="2"/>
@@ -4257,7 +4315,9 @@
       <c r="T23" s="10">
         <v>0.1</v>
       </c>
-      <c r="U23" s="10"/>
+      <c r="U23" s="10">
+        <v>0.1</v>
+      </c>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
     </row>
@@ -4348,7 +4408,7 @@
       <c r="F26" s="49">
         <v>5.5</v>
       </c>
-      <c r="G26" s="22"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="15">
         <v>9</v>
       </c>
@@ -4718,7 +4778,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M40">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lab 13: added grades.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="110">
   <si>
     <t>Nr.</t>
   </si>
@@ -64,9 +64,6 @@
     <t>L01</t>
   </si>
   <si>
-    <t>Exam problem</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -338,13 +335,28 @@
   </si>
   <si>
     <t>Bonus Proiect</t>
+  </si>
+  <si>
+    <t>Pop Julia - preda A3 in restante</t>
+  </si>
+  <si>
+    <t>Project grade without bonus</t>
+  </si>
+  <si>
+    <t>Flaviu Bompa  - preda A3 in restante</t>
+  </si>
+  <si>
+    <t>Prezentare proiecte vineri 1 iunie pe Baritiu intre 14-16</t>
+  </si>
+  <si>
+    <t>Proiect foarte bun!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -386,8 +398,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +472,48 @@
         <bgColor rgb="FFD7D7D7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFD7D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FFD7D7D7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -482,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -631,7 +691,34 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -639,6 +726,90 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -786,90 +957,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4CCCC"/>
-          <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFE7F9EF"/>
           <bgColor rgb="FFE7F9EF"/>
         </patternFill>
@@ -960,9 +1047,9 @@
     <tableColumn id="16" name="L14"/>
     <tableColumn id="17" name="Attendance"/>
     <tableColumn id="18" name="Comments"/>
-    <tableColumn id="19" name="Tema 1" dataDxfId="11"/>
-    <tableColumn id="20" name="Tema proiect final" dataDxfId="10"/>
-    <tableColumn id="21" name="Column1" dataDxfId="9"/>
+    <tableColumn id="19" name="Tema 1" dataDxfId="13"/>
+    <tableColumn id="20" name="Tema proiect final" dataDxfId="12"/>
+    <tableColumn id="21" name="Column1" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -984,16 +1071,16 @@
     <tableColumn id="11" name="Final Project"/>
     <tableColumn id="12" name="Assignments Grade"/>
     <tableColumn id="13" name="Project Grade"/>
-    <tableColumn id="14" name="Exam problem"/>
+    <tableColumn id="14" name="Project grade without bonus"/>
     <tableColumn id="15" name="Comments"/>
-    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="7"/>
-    <tableColumn id="17" name="Builder Pattern" dataDxfId="6"/>
-    <tableColumn id="18" name="DP1" dataDxfId="5"/>
-    <tableColumn id="19" name="DP2" dataDxfId="4"/>
-    <tableColumn id="20" name="DP3" dataDxfId="3"/>
-    <tableColumn id="21" name="DP4" dataDxfId="2"/>
-    <tableColumn id="22" name="DP5" dataDxfId="1"/>
-    <tableColumn id="23" name="Bonus Proiect" dataDxfId="0"/>
+    <tableColumn id="16" name="Microservicii vs SOA" dataDxfId="10"/>
+    <tableColumn id="17" name="Builder Pattern" dataDxfId="9"/>
+    <tableColumn id="18" name="DP1" dataDxfId="8"/>
+    <tableColumn id="19" name="DP2" dataDxfId="7"/>
+    <tableColumn id="20" name="DP3" dataDxfId="6"/>
+    <tableColumn id="21" name="DP4" dataDxfId="5"/>
+    <tableColumn id="22" name="DP5" dataDxfId="4"/>
+    <tableColumn id="23" name="Bonus Proiect" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1265,7 +1352,7 @@
   <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1292,58 +1379,58 @@
         <v>13</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="R1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
@@ -1358,53 +1445,55 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P2" s="56"/>
       <c r="Q2" s="17">
         <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
@@ -1420,21 +1509,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F3" s="43"/>
       <c r="G3" s="26"/>
       <c r="I3" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
@@ -1449,10 +1538,10 @@
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
@@ -1468,7 +1557,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="17"/>
@@ -1488,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -1508,53 +1597,55 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P5" s="57"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
@@ -1570,10 +1661,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
@@ -1592,10 +1683,10 @@
         <v>1</v>
       </c>
       <c r="R6" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -1612,53 +1703,55 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P7" s="57"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
@@ -1674,36 +1767,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="55"/>
       <c r="I8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="55"/>
       <c r="K8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O8" s="17"/>
       <c r="P8" s="56"/>
@@ -1713,10 +1806,10 @@
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
@@ -1732,51 +1825,53 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="51"/>
       <c r="G9" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K9" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O9" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P9" s="57"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
@@ -1792,13 +1887,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
@@ -1817,10 +1912,10 @@
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
@@ -1836,51 +1931,53 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K11" s="52"/>
       <c r="L11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P11" s="57"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T11" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
@@ -1896,45 +1993,47 @@
         <v>11</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="51"/>
       <c r="G12" s="52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="51"/>
       <c r="M12" s="51"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="O12" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P12" s="56"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T12" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
@@ -1950,53 +2049,55 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O13" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P13" s="57"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T13" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
@@ -2012,53 +2113,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="O14" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P14" s="56"/>
       <c r="Q14" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T14" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
@@ -2074,13 +2177,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
@@ -2099,10 +2202,10 @@
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T15" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
@@ -2118,53 +2221,55 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O16" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="O16" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P16" s="56"/>
       <c r="Q16" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T16" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
@@ -2180,51 +2285,53 @@
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="51"/>
+        <v>53</v>
+      </c>
+      <c r="G17" s="55"/>
       <c r="I17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M17" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N17" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="O17" s="26"/>
+        <v>53</v>
+      </c>
+      <c r="O17" s="26" t="s">
+        <v>53</v>
+      </c>
       <c r="P17" s="57"/>
       <c r="Q17" s="17">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T17" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
@@ -2240,10 +2347,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -2262,7 +2369,7 @@
         <v>1</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
@@ -2280,53 +2387,55 @@
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O19" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O19" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P19" s="57"/>
       <c r="Q19" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
@@ -2342,53 +2451,55 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O20" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P20" s="56"/>
       <c r="Q20" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T20" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -2404,7 +2515,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -2424,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="R21" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -2442,53 +2553,55 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M22" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="O22" s="17"/>
+        <v>53</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P22" s="56"/>
       <c r="Q22" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T22" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U22" s="10"/>
       <c r="V22" s="10"/>
@@ -2504,53 +2617,55 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M23" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="O23" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="O23" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="P23" s="57"/>
       <c r="Q23" s="17">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
@@ -2566,10 +2681,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -2588,7 +2703,7 @@
         <v>1</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
@@ -2606,7 +2721,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="21"/>
@@ -2626,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="R25" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
@@ -2643,44 +2758,46 @@
         <v>25</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J26" s="51"/>
       <c r="K26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M26" s="51"/>
       <c r="N26" s="51"/>
-      <c r="O26" s="17"/>
+      <c r="O26" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="P26" s="56"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="17"/>
       <c r="S26" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T26" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
@@ -2809,7 +2926,7 @@
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="19"/>
       <c r="B31" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
@@ -3071,33 +3188,33 @@
     </row>
     <row r="41" spans="1:27" ht="15" customHeight="1">
       <c r="S41" s="51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:27" ht="15" customHeight="1">
       <c r="T42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="15" customHeight="1">
       <c r="S43" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="T43" t="s">
         <v>96</v>
-      </c>
-      <c r="T43" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C27:P39 C2:F8 I2:P7 I9:P10 I8 K8:P8 C10:F11 C9:E9 C13:F26 C12:E12 I13:P25 I11:J11 L11:P11 I26 K26:L26 I12:K12 N12:P12 O26:P26">
-    <cfRule type="containsBlanks" dxfId="13" priority="4">
+    <cfRule type="containsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G7 G9:G11 G13:G16 G18:G26">
-    <cfRule type="containsBlanks" dxfId="12" priority="3">
+    <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(G2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3111,16 +3228,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
     <col min="5" max="7" width="6.85546875" customWidth="1"/>
@@ -3129,11 +3246,12 @@
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="14" width="18.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" customWidth="1"/>
+    <col min="17" max="17" width="5.140625" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" customWidth="1"/>
     <col min="19" max="20" width="7.5703125" customWidth="1"/>
     <col min="21" max="21" width="6.28515625" customWidth="1"/>
     <col min="22" max="22" width="6.7109375" customWidth="1"/>
@@ -3180,35 +3298,35 @@
       <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="S1" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="U1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
@@ -3217,7 +3335,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -3264,8 +3382,12 @@
       <c r="U2" s="10">
         <v>0.1</v>
       </c>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
+      <c r="V2" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="W2" s="62">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A3" s="19">
@@ -3273,7 +3395,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -3315,7 +3437,7 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
+      <c r="W3" s="62"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A4" s="11">
@@ -3323,7 +3445,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -3351,7 +3473,7 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
+      <c r="W4" s="62"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="19">
@@ -3359,7 +3481,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -3369,7 +3491,9 @@
       <c r="F5" s="22">
         <v>9.75</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="54">
+        <v>6</v>
+      </c>
       <c r="H5" s="23">
         <v>10</v>
       </c>
@@ -3382,7 +3506,7 @@
       <c r="K5" s="16"/>
       <c r="L5" s="16">
         <f t="shared" si="1"/>
-        <v>6.416666666666667</v>
+        <v>8.4166666666666661</v>
       </c>
       <c r="M5" s="15">
         <f t="shared" si="2"/>
@@ -3407,7 +3531,9 @@
         <v>0.1</v>
       </c>
       <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
+      <c r="W5" s="62">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A6" s="11">
@@ -3415,7 +3541,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -3443,7 +3569,7 @@
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
+      <c r="W6" s="62"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="19">
@@ -3451,7 +3577,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -3473,17 +3599,23 @@
       <c r="J7" s="23">
         <v>10</v>
       </c>
-      <c r="K7" s="16"/>
+      <c r="K7" s="60">
+        <v>10</v>
+      </c>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
         <v>9.1666666666666661</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="25"/>
+        <v>10</v>
+      </c>
+      <c r="N7" s="18">
+        <v>9.5</v>
+      </c>
+      <c r="O7" s="69" t="s">
+        <v>109</v>
+      </c>
       <c r="P7" s="10">
         <v>0.2</v>
       </c>
@@ -3500,41 +3632,49 @@
       <c r="U7" s="10">
         <v>0.1</v>
       </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
+      <c r="V7" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="W7" s="62">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>36</v>
+      <c r="B8" s="46" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="22">
         <v>5</v>
       </c>
-      <c r="F8" s="58">
+      <c r="F8" s="64">
         <v>1</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="63">
+        <v>1</v>
+      </c>
       <c r="H8" s="23">
         <v>10</v>
       </c>
       <c r="I8" s="49">
         <v>8</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="54">
+        <v>1</v>
+      </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>1.9000000000000001</v>
       </c>
       <c r="N8" s="24"/>
       <c r="O8" s="25"/>
@@ -3551,7 +3691,9 @@
         <v>0.1</v>
       </c>
       <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
+      <c r="W8" s="62">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="19">
@@ -3559,7 +3701,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -3604,8 +3746,12 @@
       <c r="U9" s="10">
         <v>0.1</v>
       </c>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
+      <c r="V9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="W9" s="62">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A10" s="11">
@@ -3613,7 +3759,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -3655,7 +3801,7 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
+      <c r="W10" s="62"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="19">
@@ -3663,7 +3809,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3714,8 +3860,12 @@
       <c r="U11" s="10">
         <v>0.1</v>
       </c>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
+      <c r="V11" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="W11" s="62">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A12" s="11">
@@ -3723,7 +3873,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -3765,7 +3915,7 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
+      <c r="W12" s="62"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="19">
@@ -3773,7 +3923,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -3817,7 +3967,9 @@
         <v>0.1</v>
       </c>
       <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
+      <c r="W13" s="62">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="11">
@@ -3825,7 +3977,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -3875,7 +4027,9 @@
         <v>0.1</v>
       </c>
       <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
+      <c r="W14" s="62">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A15" s="19">
@@ -3883,7 +4037,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -3925,7 +4079,7 @@
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
+      <c r="W15" s="62"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="11">
@@ -3933,7 +4087,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -3955,16 +4109,20 @@
       <c r="J16" s="54">
         <v>6</v>
       </c>
-      <c r="K16" s="16"/>
+      <c r="K16" s="65">
+        <v>7</v>
+      </c>
       <c r="L16" s="16">
         <f t="shared" si="1"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="M16" s="15">
         <f t="shared" si="2"/>
-        <v>2.15</v>
-      </c>
-      <c r="N16" s="18"/>
+        <v>7.0500000000000007</v>
+      </c>
+      <c r="N16" s="18">
+        <v>6.5</v>
+      </c>
       <c r="O16" s="25"/>
       <c r="P16" s="10">
         <v>0.2</v>
@@ -3983,15 +4141,17 @@
         <v>0.1</v>
       </c>
       <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
+      <c r="W16" s="62">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="19">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>45</v>
+      <c r="B17" s="68" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -4001,7 +4161,9 @@
       <c r="F17" s="22">
         <v>6.5</v>
       </c>
-      <c r="G17" s="54"/>
+      <c r="G17" s="58">
+        <v>1</v>
+      </c>
       <c r="H17" s="23">
         <v>9</v>
       </c>
@@ -4014,7 +4176,7 @@
       <c r="K17" s="16"/>
       <c r="L17" s="16">
         <f t="shared" si="1"/>
-        <v>3.8333333333333335</v>
+        <v>4.166666666666667</v>
       </c>
       <c r="M17" s="15">
         <f t="shared" si="2"/>
@@ -4031,7 +4193,9 @@
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
+      <c r="W17" s="62">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="18" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A18" s="11">
@@ -4039,7 +4203,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -4067,7 +4231,7 @@
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
+      <c r="W18" s="62"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="19">
@@ -4075,7 +4239,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -4097,16 +4261,20 @@
       <c r="J19" s="15">
         <v>9</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K19" s="16">
+        <v>8.5</v>
+      </c>
       <c r="L19" s="16">
         <f t="shared" si="1"/>
         <v>8.8333333333333339</v>
       </c>
       <c r="M19" s="15">
         <f t="shared" si="2"/>
-        <v>2.9</v>
-      </c>
-      <c r="N19" s="18"/>
+        <v>8.85</v>
+      </c>
+      <c r="N19" s="18">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="O19" s="18"/>
       <c r="P19" s="10">
         <v>0.2</v>
@@ -4121,7 +4289,9 @@
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
+      <c r="W19" s="62">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="11">
@@ -4129,7 +4299,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -4151,16 +4321,20 @@
       <c r="J20" s="15">
         <v>6</v>
       </c>
-      <c r="K20" s="16"/>
+      <c r="K20" s="16">
+        <v>5.25</v>
+      </c>
       <c r="L20" s="16">
         <f t="shared" si="1"/>
         <v>8.3333333333333339</v>
       </c>
       <c r="M20" s="15">
-        <f t="shared" si="2"/>
-        <v>2.5</v>
-      </c>
-      <c r="N20" s="18"/>
+        <f>(H20/10 +I20/10 + J20/10 + K20*7/10)</f>
+        <v>6.1749999999999998</v>
+      </c>
+      <c r="N20" s="18">
+        <v>5</v>
+      </c>
       <c r="O20" s="18"/>
       <c r="P20" s="10">
         <v>0.2</v>
@@ -4173,7 +4347,9 @@
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
+      <c r="W20" s="62">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="21" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A21" s="19">
@@ -4181,7 +4357,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -4209,7 +4385,7 @@
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
+      <c r="W21" s="62"/>
     </row>
     <row r="22" spans="1:23" ht="15.75" customHeight="1">
       <c r="A22" s="11">
@@ -4217,7 +4393,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -4245,7 +4421,7 @@
         <v>7.666666666666667</v>
       </c>
       <c r="M22" s="15">
-        <f t="shared" si="2"/>
+        <f>(H22/10 +I22/10 + J22/10 + K22*7/10)</f>
         <v>2</v>
       </c>
       <c r="N22" s="18"/>
@@ -4258,8 +4434,12 @@
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
+      <c r="V22" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="W22" s="62">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="19">
@@ -4267,7 +4447,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -4289,16 +4469,20 @@
       <c r="J23" s="15">
         <v>6.5</v>
       </c>
-      <c r="K23" s="16"/>
+      <c r="K23" s="16">
+        <v>8.5</v>
+      </c>
       <c r="L23" s="16">
         <f t="shared" si="1"/>
         <v>9.25</v>
       </c>
       <c r="M23" s="15">
         <f t="shared" si="2"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="N23" s="18"/>
+        <v>8.25</v>
+      </c>
+      <c r="N23" s="18">
+        <v>7.75</v>
+      </c>
       <c r="O23" s="18"/>
       <c r="P23" s="10">
         <v>0.2</v>
@@ -4318,8 +4502,12 @@
       <c r="U23" s="10">
         <v>0.1</v>
       </c>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
+      <c r="V23" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="W23" s="62">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="24" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A24" s="11">
@@ -4327,7 +4515,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -4355,7 +4543,7 @@
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
+      <c r="W24" s="62"/>
     </row>
     <row r="25" spans="1:23" ht="15.75" hidden="1" customHeight="1">
       <c r="A25" s="19">
@@ -4363,7 +4551,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -4391,14 +4579,14 @@
       <c r="T25" s="10"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
+      <c r="W25" s="62"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="18">
         <v>23</v>
       </c>
-      <c r="B26" s="29" t="s">
-        <v>88</v>
+      <c r="B26" s="67" t="s">
+        <v>87</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -4408,22 +4596,26 @@
       <c r="F26" s="49">
         <v>5.5</v>
       </c>
-      <c r="G26" s="54"/>
+      <c r="G26" s="63">
+        <v>1</v>
+      </c>
       <c r="H26" s="15">
         <v>9</v>
       </c>
       <c r="I26" s="49">
         <v>7</v>
       </c>
-      <c r="J26" s="54"/>
+      <c r="J26" s="54">
+        <v>5</v>
+      </c>
       <c r="K26" s="16"/>
       <c r="L26" s="16">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>4.583333333333333</v>
       </c>
       <c r="M26" s="23">
         <f t="shared" si="2"/>
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -4434,7 +4626,7 @@
       <c r="T26" s="10"/>
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
+      <c r="W26" s="62"/>
     </row>
     <row r="27" spans="1:23" ht="15.75" customHeight="1">
       <c r="A27" s="31"/>
@@ -4503,7 +4695,7 @@
       <c r="N29" s="18"/>
       <c r="O29" s="18"/>
       <c r="P29" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
@@ -4765,10 +4957,10 @@
     </row>
     <row r="40" spans="1:23" ht="15" customHeight="1">
       <c r="P40" s="53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
@@ -4776,9 +4968,28 @@
       <c r="V40" s="10"/>
       <c r="W40" s="10"/>
     </row>
+    <row r="41" spans="1:23" ht="15" customHeight="1">
+      <c r="P41" s="59"/>
+    </row>
+    <row r="42" spans="1:23" ht="15" customHeight="1">
+      <c r="B42" t="s">
+        <v>105</v>
+      </c>
+      <c r="K42" s="10"/>
+    </row>
+    <row r="43" spans="1:23" ht="15" customHeight="1">
+      <c r="B43" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="15" customHeight="1">
+      <c r="B44" s="66" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="L2:M40">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>